<commit_message>
no run time errors, only failing tests. However, input data needs to be revised to increase code coverage, and new run-time errors may appear there.
</commit_message>
<xml_diff>
--- a/test_constraints.xlsx
+++ b/test_constraints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HumeD\PycharmProjects\Data_Profile_Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332346E6-3BA0-4946-846C-AB5A22BD0EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9CD0B0-D824-42B6-9619-AAA6C4B40301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{D2E9D144-5D6F-4AC1-9DA3-D4FF634D9598}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{D2E9D144-5D6F-4AC1-9DA3-D4FF634D9598}"/>
   </bookViews>
   <sheets>
     <sheet name="Constraint Set Definitions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Constraint Types" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="171">
   <si>
     <t>Constraint_Set_Name</t>
   </si>
@@ -534,6 +533,24 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>unique_id,dim1,dim2,val1,val2</t>
+  </si>
+  <si>
+    <t>int,String,String,int,int</t>
+  </si>
+  <si>
+    <t>int,int,int,int,int</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>a,b,c,d,e</t>
+  </si>
+  <si>
+    <t>0.25 &lt;= P[0] x S[0] &lt;= 0.75</t>
   </si>
 </sst>
 </file>
@@ -603,8 +620,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -915,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8623B9B9-CDA9-468A-BDFA-05B32D11770D}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,7 +1414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B3F463-1905-4B9F-9CAD-CAAB02DF2A5C}">
   <dimension ref="A1:BN18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
@@ -2199,10 +2257,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E86614-3B97-43D1-B6C4-36CEB2305CDA}">
-  <dimension ref="A1:K178"/>
+  <dimension ref="A1:K179"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,19 +2600,19 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>150</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>168</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="H10" t="s">
         <v>61</v>
@@ -2577,13 +2635,13 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>150</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
         <v>61</v>
@@ -2591,8 +2649,8 @@
       <c r="G11" t="s">
         <v>61</v>
       </c>
-      <c r="H11">
-        <v>0</v>
+      <c r="H11" t="s">
+        <v>61</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -2612,13 +2670,13 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
         <v>150</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
         <v>61</v>
@@ -2647,22 +2705,22 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>150</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s">
         <v>61</v>
       </c>
-      <c r="H13" t="s">
-        <v>61</v>
+      <c r="H13">
+        <v>0</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -2676,22 +2734,22 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G14" t="s">
         <v>61</v>
@@ -2700,10 +2758,10 @@
         <v>61</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -2717,13 +2775,13 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
         <v>151</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F15" t="s">
         <v>61</v>
@@ -2731,8 +2789,8 @@
       <c r="G15" t="s">
         <v>61</v>
       </c>
-      <c r="H15">
-        <v>0</v>
+      <c r="H15" t="s">
+        <v>61</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -2752,13 +2810,13 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
         <v>151</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" t="s">
         <v>61</v>
@@ -2787,22 +2845,22 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>151</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="G17" t="s">
         <v>61</v>
       </c>
-      <c r="H17" t="s">
-        <v>61</v>
+      <c r="H17">
+        <v>0</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -2816,22 +2874,22 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G18" t="s">
         <v>61</v>
@@ -2840,10 +2898,10 @@
         <v>61</v>
       </c>
       <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>48</v>
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -2857,13 +2915,13 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
         <v>150</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
         <v>61</v>
@@ -2871,8 +2929,8 @@
       <c r="G19" t="s">
         <v>61</v>
       </c>
-      <c r="H19">
-        <v>0</v>
+      <c r="H19" t="s">
+        <v>61</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2892,13 +2950,13 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
         <v>150</v>
       </c>
       <c r="E20" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F20" t="s">
         <v>61</v>
@@ -2927,22 +2985,22 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
         <v>150</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
         <v>61</v>
       </c>
-      <c r="H21" t="s">
-        <v>61</v>
+      <c r="H21">
+        <v>0</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -2962,19 +3020,19 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
         <v>150</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F22" t="s">
         <v>46</v>
       </c>
-      <c r="G22">
-        <v>2</v>
+      <c r="G22" t="s">
+        <v>61</v>
       </c>
       <c r="H22" t="s">
         <v>61</v>
@@ -2997,19 +3055,22 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
         <v>150</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" t="s">
         <v>46</v>
       </c>
-      <c r="H23">
+      <c r="G23">
         <v>2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>61</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -3029,16 +3090,19 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
         <v>150</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
         <v>46</v>
+      </c>
+      <c r="G24" t="s">
+        <v>162</v>
       </c>
       <c r="H24">
         <v>2</v>
@@ -3061,16 +3125,19 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
         <v>150</v>
       </c>
       <c r="E25" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="F25" t="s">
         <v>46</v>
+      </c>
+      <c r="G25" t="s">
+        <v>162</v>
       </c>
       <c r="H25">
         <v>2</v>
@@ -3093,16 +3160,19 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
         <v>150</v>
       </c>
       <c r="E26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F26" t="s">
         <v>46</v>
+      </c>
+      <c r="G26" t="s">
+        <v>162</v>
       </c>
       <c r="H26">
         <v>2</v>
@@ -3125,16 +3195,19 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
         <v>150</v>
       </c>
       <c r="E27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F27" t="s">
         <v>46</v>
+      </c>
+      <c r="G27" t="s">
+        <v>162</v>
       </c>
       <c r="H27">
         <v>2</v>
@@ -3157,16 +3230,19 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
         <v>150</v>
       </c>
       <c r="E28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F28" t="s">
         <v>46</v>
+      </c>
+      <c r="G28" t="s">
+        <v>162</v>
       </c>
       <c r="H28">
         <v>2</v>
@@ -3189,17 +3265,20 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
         <v>150</v>
       </c>
       <c r="E29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F29" t="s">
         <v>46</v>
       </c>
+      <c r="G29" t="s">
+        <v>162</v>
+      </c>
       <c r="H29">
         <v>2</v>
       </c>
@@ -3215,25 +3294,28 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E30" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G30" t="s">
-        <v>61</v>
+        <v>162</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -3253,18 +3335,21 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
         <v>151</v>
       </c>
       <c r="E31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="F31" t="s">
+        <v>61</v>
       </c>
       <c r="G31" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" t="s">
         <v>61</v>
       </c>
       <c r="I31">
@@ -3285,19 +3370,22 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
         <v>151</v>
       </c>
       <c r="E32" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
       <c r="G32" t="s">
         <v>61</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -3317,22 +3405,22 @@
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
         <v>151</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" t="s">
-        <v>46</v>
+        <v>128</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
       </c>
       <c r="G33" t="s">
         <v>61</v>
       </c>
-      <c r="H33" t="s">
-        <v>61</v>
+      <c r="H33">
+        <v>2</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -3352,16 +3440,19 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D34" t="s">
         <v>151</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F34" t="s">
         <v>46</v>
+      </c>
+      <c r="G34" t="s">
+        <v>61</v>
       </c>
       <c r="H34" t="s">
         <v>61</v>
@@ -3384,19 +3475,22 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D35" t="s">
         <v>151</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F35" t="s">
         <v>46</v>
       </c>
-      <c r="H35">
-        <v>2</v>
+      <c r="G35" t="s">
+        <v>162</v>
+      </c>
+      <c r="H35" t="s">
+        <v>61</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -3416,16 +3510,19 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D36" t="s">
         <v>151</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F36" t="s">
         <v>46</v>
+      </c>
+      <c r="G36" t="s">
+        <v>162</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3448,16 +3545,19 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D37" t="s">
         <v>151</v>
       </c>
       <c r="E37" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="F37" t="s">
         <v>46</v>
+      </c>
+      <c r="G37" t="s">
+        <v>162</v>
       </c>
       <c r="H37">
         <v>2</v>
@@ -3480,16 +3580,19 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D38" t="s">
         <v>151</v>
       </c>
       <c r="E38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F38" t="s">
         <v>46</v>
+      </c>
+      <c r="G38" t="s">
+        <v>162</v>
       </c>
       <c r="H38">
         <v>2</v>
@@ -3512,16 +3615,19 @@
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D39" t="s">
         <v>151</v>
       </c>
       <c r="E39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F39" t="s">
         <v>46</v>
+      </c>
+      <c r="G39" t="s">
+        <v>162</v>
       </c>
       <c r="H39">
         <v>2</v>
@@ -3544,16 +3650,19 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D40" t="s">
         <v>151</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F40" t="s">
         <v>46</v>
+      </c>
+      <c r="G40" t="s">
+        <v>162</v>
       </c>
       <c r="H40">
         <v>2</v>
@@ -3576,17 +3685,20 @@
         <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D41" t="s">
         <v>151</v>
       </c>
       <c r="E41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F41" t="s">
         <v>46</v>
       </c>
+      <c r="G41" t="s">
+        <v>162</v>
+      </c>
       <c r="H41">
         <v>2</v>
       </c>
@@ -3602,31 +3714,34 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="D42" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E42" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="F42" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G42" t="s">
-        <v>61</v>
+        <v>162</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
       </c>
       <c r="I42">
-        <v>1</v>
-      </c>
-      <c r="J42">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>48</v>
       </c>
       <c r="K42">
         <v>1</v>
@@ -3640,18 +3755,21 @@
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D43" t="s">
         <v>150</v>
       </c>
       <c r="E43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="F43" t="s">
+        <v>61</v>
       </c>
       <c r="G43" t="s">
+        <v>61</v>
+      </c>
+      <c r="H43" t="s">
         <v>61</v>
       </c>
       <c r="I43">
@@ -3672,19 +3790,22 @@
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D44" t="s">
         <v>150</v>
       </c>
       <c r="E44" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F44">
         <v>0</v>
       </c>
       <c r="G44" t="s">
         <v>61</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
       </c>
       <c r="I44">
         <v>1</v>
@@ -3704,22 +3825,22 @@
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D45" t="s">
         <v>150</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" t="s">
-        <v>46</v>
+        <v>128</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
       </c>
       <c r="G45" t="s">
         <v>61</v>
       </c>
-      <c r="H45" t="s">
-        <v>61</v>
+      <c r="H45">
+        <v>2</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -3739,16 +3860,19 @@
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D46" t="s">
         <v>150</v>
       </c>
       <c r="E46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F46" t="s">
         <v>46</v>
+      </c>
+      <c r="G46" t="s">
+        <v>61</v>
       </c>
       <c r="H46" t="s">
         <v>61</v>
@@ -3771,19 +3895,22 @@
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D47" t="s">
         <v>150</v>
       </c>
       <c r="E47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F47" t="s">
         <v>46</v>
       </c>
-      <c r="H47">
-        <v>2</v>
+      <c r="G47" t="s">
+        <v>162</v>
+      </c>
+      <c r="H47" t="s">
+        <v>61</v>
       </c>
       <c r="I47">
         <v>1</v>
@@ -3803,16 +3930,19 @@
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D48" t="s">
         <v>150</v>
       </c>
       <c r="E48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F48" t="s">
         <v>46</v>
+      </c>
+      <c r="G48" t="s">
+        <v>162</v>
       </c>
       <c r="H48">
         <v>2</v>
@@ -3835,16 +3965,19 @@
         <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D49" t="s">
         <v>150</v>
       </c>
       <c r="E49" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="F49" t="s">
         <v>46</v>
+      </c>
+      <c r="G49" t="s">
+        <v>162</v>
       </c>
       <c r="H49">
         <v>2</v>
@@ -3867,16 +4000,19 @@
         <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D50" t="s">
         <v>150</v>
       </c>
       <c r="E50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F50" t="s">
         <v>46</v>
+      </c>
+      <c r="G50" t="s">
+        <v>162</v>
       </c>
       <c r="H50">
         <v>2</v>
@@ -3899,16 +4035,19 @@
         <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D51" t="s">
         <v>150</v>
       </c>
       <c r="E51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F51" t="s">
         <v>46</v>
+      </c>
+      <c r="G51" t="s">
+        <v>162</v>
       </c>
       <c r="H51">
         <v>2</v>
@@ -3931,17 +4070,20 @@
         <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D52" t="s">
         <v>150</v>
       </c>
       <c r="E52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F52" t="s">
         <v>46</v>
       </c>
+      <c r="G52" t="s">
+        <v>162</v>
+      </c>
       <c r="H52">
         <v>2</v>
       </c>
@@ -3957,22 +4099,25 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B53">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F53" t="s">
         <v>46</v>
+      </c>
+      <c r="G53" t="s">
+        <v>162</v>
       </c>
       <c r="H53">
         <v>2</v>
@@ -3995,19 +4140,22 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D54" t="s">
         <v>151</v>
       </c>
       <c r="E54" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="F54" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G54" t="s">
-        <v>61</v>
+        <v>162</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
       </c>
       <c r="I54">
         <v>1</v>
@@ -4027,18 +4175,21 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D55" t="s">
         <v>151</v>
       </c>
       <c r="E55" t="s">
-        <v>32</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="F55" t="s">
+        <v>61</v>
       </c>
       <c r="G55" t="s">
+        <v>61</v>
+      </c>
+      <c r="H55" t="s">
         <v>61</v>
       </c>
       <c r="I55">
@@ -4059,19 +4210,22 @@
         <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D56" t="s">
         <v>151</v>
       </c>
       <c r="E56" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F56">
         <v>0</v>
       </c>
       <c r="G56" t="s">
         <v>61</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
       </c>
       <c r="I56">
         <v>1</v>
@@ -4091,22 +4245,22 @@
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D57" t="s">
         <v>151</v>
       </c>
       <c r="E57" t="s">
-        <v>33</v>
-      </c>
-      <c r="F57" t="s">
-        <v>46</v>
+        <v>128</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
       </c>
       <c r="G57" t="s">
         <v>61</v>
       </c>
-      <c r="H57" t="s">
-        <v>61</v>
+      <c r="H57">
+        <v>2</v>
       </c>
       <c r="I57">
         <v>1</v>
@@ -4126,16 +4280,19 @@
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D58" t="s">
         <v>151</v>
       </c>
       <c r="E58" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F58" t="s">
         <v>46</v>
+      </c>
+      <c r="G58" t="s">
+        <v>61</v>
       </c>
       <c r="H58" t="s">
         <v>61</v>
@@ -4158,19 +4315,22 @@
         <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D59" t="s">
         <v>151</v>
       </c>
       <c r="E59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F59" t="s">
         <v>46</v>
       </c>
-      <c r="H59">
-        <v>2</v>
+      <c r="G59" t="s">
+        <v>162</v>
+      </c>
+      <c r="H59" t="s">
+        <v>61</v>
       </c>
       <c r="I59">
         <v>1</v>
@@ -4190,16 +4350,19 @@
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D60" t="s">
         <v>151</v>
       </c>
       <c r="E60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F60" t="s">
         <v>46</v>
+      </c>
+      <c r="G60" t="s">
+        <v>162</v>
       </c>
       <c r="H60">
         <v>2</v>
@@ -4222,16 +4385,19 @@
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D61" t="s">
         <v>151</v>
       </c>
       <c r="E61" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="F61" t="s">
         <v>46</v>
+      </c>
+      <c r="G61" t="s">
+        <v>162</v>
       </c>
       <c r="H61">
         <v>2</v>
@@ -4254,16 +4420,19 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D62" t="s">
         <v>151</v>
       </c>
       <c r="E62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F62" t="s">
         <v>46</v>
+      </c>
+      <c r="G62" t="s">
+        <v>162</v>
       </c>
       <c r="H62">
         <v>2</v>
@@ -4286,16 +4455,19 @@
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D63" t="s">
         <v>151</v>
       </c>
       <c r="E63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F63" t="s">
         <v>46</v>
+      </c>
+      <c r="G63" t="s">
+        <v>162</v>
       </c>
       <c r="H63">
         <v>2</v>
@@ -4318,16 +4490,19 @@
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D64" t="s">
         <v>151</v>
       </c>
       <c r="E64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F64" t="s">
         <v>46</v>
+      </c>
+      <c r="G64" t="s">
+        <v>162</v>
       </c>
       <c r="H64">
         <v>2</v>
@@ -4350,17 +4525,20 @@
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D65" t="s">
         <v>151</v>
       </c>
       <c r="E65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F65" t="s">
         <v>46</v>
       </c>
+      <c r="G65" t="s">
+        <v>162</v>
+      </c>
       <c r="H65">
         <v>2</v>
       </c>
@@ -4376,25 +4554,28 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B66">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D66" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E66" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="F66" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G66" t="s">
-        <v>61</v>
+        <v>162</v>
+      </c>
+      <c r="H66">
+        <v>2</v>
       </c>
       <c r="I66">
         <v>1</v>
@@ -4414,18 +4595,21 @@
         <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D67" t="s">
         <v>150</v>
       </c>
       <c r="E67" t="s">
-        <v>32</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="F67" t="s">
+        <v>61</v>
       </c>
       <c r="G67" t="s">
+        <v>61</v>
+      </c>
+      <c r="H67" t="s">
         <v>61</v>
       </c>
       <c r="I67">
@@ -4446,19 +4630,22 @@
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D68" t="s">
         <v>150</v>
       </c>
       <c r="E68" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F68">
         <v>0</v>
       </c>
       <c r="G68" t="s">
         <v>61</v>
+      </c>
+      <c r="H68">
+        <v>2</v>
       </c>
       <c r="I68">
         <v>1</v>
@@ -4478,22 +4665,22 @@
         <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D69" t="s">
         <v>150</v>
       </c>
       <c r="E69" t="s">
-        <v>33</v>
-      </c>
-      <c r="F69" t="s">
-        <v>46</v>
+        <v>128</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
       </c>
       <c r="G69" t="s">
         <v>61</v>
       </c>
-      <c r="H69" t="s">
-        <v>61</v>
+      <c r="H69">
+        <v>2</v>
       </c>
       <c r="I69">
         <v>1</v>
@@ -4513,16 +4700,19 @@
         <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D70" t="s">
         <v>150</v>
       </c>
       <c r="E70" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F70" t="s">
         <v>46</v>
+      </c>
+      <c r="G70" t="s">
+        <v>61</v>
       </c>
       <c r="H70" t="s">
         <v>61</v>
@@ -4545,19 +4735,22 @@
         <v>9</v>
       </c>
       <c r="C71" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D71" t="s">
         <v>150</v>
       </c>
       <c r="E71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F71" t="s">
         <v>46</v>
       </c>
-      <c r="H71">
-        <v>2</v>
+      <c r="G71" t="s">
+        <v>162</v>
+      </c>
+      <c r="H71" t="s">
+        <v>61</v>
       </c>
       <c r="I71">
         <v>1</v>
@@ -4577,16 +4770,19 @@
         <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D72" t="s">
         <v>150</v>
       </c>
       <c r="E72" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F72" t="s">
         <v>46</v>
+      </c>
+      <c r="G72" t="s">
+        <v>162</v>
       </c>
       <c r="H72">
         <v>2</v>
@@ -4609,16 +4805,19 @@
         <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D73" t="s">
         <v>150</v>
       </c>
       <c r="E73" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="F73" t="s">
         <v>46</v>
+      </c>
+      <c r="G73" t="s">
+        <v>162</v>
       </c>
       <c r="H73">
         <v>2</v>
@@ -4641,16 +4840,19 @@
         <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D74" t="s">
         <v>150</v>
       </c>
       <c r="E74" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F74" t="s">
         <v>46</v>
+      </c>
+      <c r="G74" t="s">
+        <v>162</v>
       </c>
       <c r="H74">
         <v>2</v>
@@ -4673,16 +4875,19 @@
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D75" t="s">
         <v>150</v>
       </c>
       <c r="E75" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F75" t="s">
         <v>46</v>
+      </c>
+      <c r="G75" t="s">
+        <v>162</v>
       </c>
       <c r="H75">
         <v>2</v>
@@ -4705,16 +4910,19 @@
         <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D76" t="s">
         <v>150</v>
       </c>
       <c r="E76" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F76" t="s">
         <v>46</v>
+      </c>
+      <c r="G76" t="s">
+        <v>162</v>
       </c>
       <c r="H76">
         <v>2</v>
@@ -4737,17 +4945,20 @@
         <v>9</v>
       </c>
       <c r="C77" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D77" t="s">
         <v>150</v>
       </c>
       <c r="E77" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F77" t="s">
         <v>46</v>
       </c>
+      <c r="G77" t="s">
+        <v>162</v>
+      </c>
       <c r="H77">
         <v>2</v>
       </c>
@@ -4763,25 +4974,28 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B78">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C78" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D78" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E78" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="F78" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G78" t="s">
-        <v>61</v>
+        <v>162</v>
+      </c>
+      <c r="H78">
+        <v>2</v>
       </c>
       <c r="I78">
         <v>1</v>
@@ -4801,18 +5015,21 @@
         <v>10</v>
       </c>
       <c r="C79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D79" t="s">
         <v>151</v>
       </c>
       <c r="E79" t="s">
-        <v>32</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="F79" t="s">
+        <v>61</v>
       </c>
       <c r="G79" t="s">
+        <v>61</v>
+      </c>
+      <c r="H79" t="s">
         <v>61</v>
       </c>
       <c r="I79">
@@ -4833,19 +5050,22 @@
         <v>10</v>
       </c>
       <c r="C80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D80" t="s">
         <v>151</v>
       </c>
       <c r="E80" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F80">
         <v>0</v>
       </c>
       <c r="G80" t="s">
         <v>61</v>
+      </c>
+      <c r="H80">
+        <v>2</v>
       </c>
       <c r="I80">
         <v>1</v>
@@ -4865,22 +5085,22 @@
         <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D81" t="s">
         <v>151</v>
       </c>
       <c r="E81" t="s">
-        <v>33</v>
-      </c>
-      <c r="F81" t="s">
-        <v>46</v>
+        <v>128</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
       </c>
       <c r="G81" t="s">
         <v>61</v>
       </c>
-      <c r="H81" t="s">
-        <v>61</v>
+      <c r="H81">
+        <v>2</v>
       </c>
       <c r="I81">
         <v>1</v>
@@ -4900,16 +5120,19 @@
         <v>10</v>
       </c>
       <c r="C82" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D82" t="s">
         <v>151</v>
       </c>
       <c r="E82" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F82" t="s">
         <v>46</v>
+      </c>
+      <c r="G82" t="s">
+        <v>61</v>
       </c>
       <c r="H82" t="s">
         <v>61</v>
@@ -4932,19 +5155,22 @@
         <v>10</v>
       </c>
       <c r="C83" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D83" t="s">
         <v>151</v>
       </c>
       <c r="E83" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F83" t="s">
         <v>46</v>
       </c>
-      <c r="H83">
-        <v>2</v>
+      <c r="G83" t="s">
+        <v>162</v>
+      </c>
+      <c r="H83" t="s">
+        <v>61</v>
       </c>
       <c r="I83">
         <v>1</v>
@@ -4964,16 +5190,19 @@
         <v>10</v>
       </c>
       <c r="C84" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D84" t="s">
         <v>151</v>
       </c>
       <c r="E84" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F84" t="s">
         <v>46</v>
+      </c>
+      <c r="G84" t="s">
+        <v>162</v>
       </c>
       <c r="H84">
         <v>2</v>
@@ -4996,16 +5225,19 @@
         <v>10</v>
       </c>
       <c r="C85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D85" t="s">
         <v>151</v>
       </c>
       <c r="E85" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="F85" t="s">
         <v>46</v>
+      </c>
+      <c r="G85" t="s">
+        <v>162</v>
       </c>
       <c r="H85">
         <v>2</v>
@@ -5028,16 +5260,19 @@
         <v>10</v>
       </c>
       <c r="C86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D86" t="s">
         <v>151</v>
       </c>
       <c r="E86" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F86" t="s">
         <v>46</v>
+      </c>
+      <c r="G86" t="s">
+        <v>162</v>
       </c>
       <c r="H86">
         <v>2</v>
@@ -5060,16 +5295,19 @@
         <v>10</v>
       </c>
       <c r="C87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D87" t="s">
         <v>151</v>
       </c>
       <c r="E87" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F87" t="s">
         <v>46</v>
+      </c>
+      <c r="G87" t="s">
+        <v>162</v>
       </c>
       <c r="H87">
         <v>2</v>
@@ -5092,16 +5330,19 @@
         <v>10</v>
       </c>
       <c r="C88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D88" t="s">
         <v>151</v>
       </c>
       <c r="E88" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F88" t="s">
         <v>46</v>
+      </c>
+      <c r="G88" t="s">
+        <v>162</v>
       </c>
       <c r="H88">
         <v>2</v>
@@ -5124,17 +5365,20 @@
         <v>10</v>
       </c>
       <c r="C89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D89" t="s">
         <v>151</v>
       </c>
       <c r="E89" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F89" t="s">
         <v>46</v>
       </c>
+      <c r="G89" t="s">
+        <v>162</v>
+      </c>
       <c r="H89">
         <v>2</v>
       </c>
@@ -5150,22 +5394,34 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B90">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C90" t="s">
+        <v>98</v>
       </c>
       <c r="D90" t="s">
         <v>151</v>
       </c>
       <c r="E90" t="s">
-        <v>62</v>
-      </c>
-      <c r="I90" t="s">
-        <v>61</v>
-      </c>
-      <c r="J90" t="s">
-        <v>61</v>
+        <v>127</v>
+      </c>
+      <c r="F90" t="s">
+        <v>46</v>
+      </c>
+      <c r="G90" t="s">
+        <v>162</v>
+      </c>
+      <c r="H90">
+        <v>2</v>
+      </c>
+      <c r="I90">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
       </c>
       <c r="K90">
         <v>1</v>
@@ -5173,10 +5429,10 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B91">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D91" t="s">
         <v>151</v>
@@ -5184,6 +5440,15 @@
       <c r="E91" t="s">
         <v>62</v>
       </c>
+      <c r="F91" t="s">
+        <v>61</v>
+      </c>
+      <c r="G91" t="s">
+        <v>166</v>
+      </c>
+      <c r="H91" t="s">
+        <v>61</v>
+      </c>
       <c r="I91" t="s">
         <v>61</v>
       </c>
@@ -5196,10 +5461,10 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B92">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D92" t="s">
         <v>151</v>
@@ -5207,6 +5472,15 @@
       <c r="E92" t="s">
         <v>62</v>
       </c>
+      <c r="F92" t="s">
+        <v>61</v>
+      </c>
+      <c r="G92" t="s">
+        <v>166</v>
+      </c>
+      <c r="H92" t="s">
+        <v>61</v>
+      </c>
       <c r="I92" t="s">
         <v>61</v>
       </c>
@@ -5219,10 +5493,10 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="B93">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D93" t="s">
         <v>151</v>
@@ -5230,6 +5504,15 @@
       <c r="E93" t="s">
         <v>62</v>
       </c>
+      <c r="F93" t="s">
+        <v>61</v>
+      </c>
+      <c r="G93" t="s">
+        <v>166</v>
+      </c>
+      <c r="H93" t="s">
+        <v>61</v>
+      </c>
       <c r="I93" t="s">
         <v>61</v>
       </c>
@@ -5242,16 +5525,31 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="B94">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E94" t="s">
-        <v>37</v>
+        <v>132</v>
+      </c>
+      <c r="F94" t="s">
+        <v>61</v>
+      </c>
+      <c r="G94" t="s">
+        <v>167</v>
+      </c>
+      <c r="H94" t="s">
+        <v>61</v>
+      </c>
+      <c r="I94" t="s">
+        <v>61</v>
+      </c>
+      <c r="J94" t="s">
+        <v>61</v>
       </c>
       <c r="K94">
         <v>1</v>
@@ -5259,27 +5557,48 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B95">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C95" t="s">
+        <v>170</v>
       </c>
       <c r="D95" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E95" t="s">
         <v>37</v>
       </c>
+      <c r="F95" t="s">
+        <v>61</v>
+      </c>
+      <c r="G95" t="s">
+        <v>61</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0.25</v>
+      </c>
+      <c r="J95">
+        <v>0.75</v>
+      </c>
       <c r="K95">
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B96">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="C96" t="s">
+        <v>170</v>
       </c>
       <c r="D96" t="s">
         <v>151</v>
@@ -5287,22 +5606,55 @@
       <c r="E96" t="s">
         <v>37</v>
       </c>
+      <c r="F96" t="s">
+        <v>61</v>
+      </c>
+      <c r="G96" t="s">
+        <v>61</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0.25</v>
+      </c>
+      <c r="J96">
+        <v>0.75</v>
+      </c>
       <c r="K96">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="B97">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C97" t="s">
+        <v>170</v>
       </c>
       <c r="D97" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E97" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="F97" t="s">
+        <v>61</v>
+      </c>
+      <c r="G97" t="s">
+        <v>61</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0.25</v>
+      </c>
+      <c r="J97">
+        <v>0.75</v>
       </c>
       <c r="K97">
         <v>1</v>
@@ -5319,7 +5671,22 @@
         <v>152</v>
       </c>
       <c r="E98" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="F98" t="s">
+        <v>168</v>
+      </c>
+      <c r="G98" t="s">
+        <v>61</v>
+      </c>
+      <c r="H98">
+        <v>70</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
       </c>
       <c r="K98">
         <v>1</v>
@@ -5336,7 +5703,22 @@
         <v>152</v>
       </c>
       <c r="E99" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="F99" t="s">
+        <v>168</v>
+      </c>
+      <c r="G99" t="s">
+        <v>162</v>
+      </c>
+      <c r="H99">
+        <v>70</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
       </c>
       <c r="K99">
         <v>1</v>
@@ -5353,7 +5735,22 @@
         <v>152</v>
       </c>
       <c r="E100" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="F100" t="s">
+        <v>168</v>
+      </c>
+      <c r="G100" t="s">
+        <v>162</v>
+      </c>
+      <c r="H100">
+        <v>70</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
       </c>
       <c r="K100">
         <v>1</v>
@@ -5370,7 +5767,22 @@
         <v>152</v>
       </c>
       <c r="E101" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="F101" t="s">
+        <v>168</v>
+      </c>
+      <c r="G101" t="s">
+        <v>162</v>
+      </c>
+      <c r="H101">
+        <v>70</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
       </c>
       <c r="K101">
         <v>1</v>
@@ -5387,7 +5799,22 @@
         <v>152</v>
       </c>
       <c r="E102" t="s">
-        <v>128</v>
+        <v>32</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102" t="s">
+        <v>61</v>
+      </c>
+      <c r="H102">
+        <v>70</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
       </c>
       <c r="K102">
         <v>1</v>
@@ -5404,7 +5831,22 @@
         <v>152</v>
       </c>
       <c r="E103" t="s">
-        <v>33</v>
+        <v>128</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103" t="s">
+        <v>61</v>
+      </c>
+      <c r="H103">
+        <v>70</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
       </c>
       <c r="K103">
         <v>1</v>
@@ -5421,7 +5863,22 @@
         <v>152</v>
       </c>
       <c r="E104" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="F104" t="s">
+        <v>168</v>
+      </c>
+      <c r="G104" t="s">
+        <v>61</v>
+      </c>
+      <c r="H104">
+        <v>70</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
       </c>
       <c r="K104">
         <v>1</v>
@@ -5438,7 +5895,22 @@
         <v>152</v>
       </c>
       <c r="E105" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="F105" t="s">
+        <v>168</v>
+      </c>
+      <c r="G105" t="s">
+        <v>162</v>
+      </c>
+      <c r="H105">
+        <v>70</v>
+      </c>
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
       </c>
       <c r="K105">
         <v>1</v>
@@ -5455,7 +5927,22 @@
         <v>152</v>
       </c>
       <c r="E106" t="s">
-        <v>117</v>
+        <v>36</v>
+      </c>
+      <c r="F106" t="s">
+        <v>168</v>
+      </c>
+      <c r="G106" t="s">
+        <v>162</v>
+      </c>
+      <c r="H106">
+        <v>70</v>
+      </c>
+      <c r="I106">
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
       </c>
       <c r="K106">
         <v>1</v>
@@ -5472,7 +5959,22 @@
         <v>152</v>
       </c>
       <c r="E107" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="F107" t="s">
+        <v>168</v>
+      </c>
+      <c r="G107" t="s">
+        <v>162</v>
+      </c>
+      <c r="H107">
+        <v>70</v>
+      </c>
+      <c r="I107">
+        <v>0</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
       </c>
       <c r="K107">
         <v>1</v>
@@ -5489,7 +5991,22 @@
         <v>152</v>
       </c>
       <c r="E108" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="F108" t="s">
+        <v>168</v>
+      </c>
+      <c r="G108" t="s">
+        <v>162</v>
+      </c>
+      <c r="H108">
+        <v>70</v>
+      </c>
+      <c r="I108">
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
       </c>
       <c r="K108">
         <v>1</v>
@@ -5506,7 +6023,22 @@
         <v>152</v>
       </c>
       <c r="E109" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="F109" t="s">
+        <v>168</v>
+      </c>
+      <c r="G109" t="s">
+        <v>162</v>
+      </c>
+      <c r="H109">
+        <v>70</v>
+      </c>
+      <c r="I109">
+        <v>0</v>
+      </c>
+      <c r="J109">
+        <v>0</v>
       </c>
       <c r="K109">
         <v>1</v>
@@ -5523,7 +6055,22 @@
         <v>152</v>
       </c>
       <c r="E110" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="F110" t="s">
+        <v>168</v>
+      </c>
+      <c r="G110" t="s">
+        <v>162</v>
+      </c>
+      <c r="H110">
+        <v>70</v>
+      </c>
+      <c r="I110">
+        <v>0</v>
+      </c>
+      <c r="J110">
+        <v>0</v>
       </c>
       <c r="K110">
         <v>1</v>
@@ -5540,7 +6087,22 @@
         <v>152</v>
       </c>
       <c r="E111" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="F111" t="s">
+        <v>168</v>
+      </c>
+      <c r="G111" t="s">
+        <v>162</v>
+      </c>
+      <c r="H111">
+        <v>70</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111">
+        <v>0</v>
       </c>
       <c r="K111">
         <v>1</v>
@@ -5557,7 +6119,22 @@
         <v>152</v>
       </c>
       <c r="E112" t="s">
-        <v>123</v>
+        <v>122</v>
+      </c>
+      <c r="F112" t="s">
+        <v>168</v>
+      </c>
+      <c r="G112" t="s">
+        <v>162</v>
+      </c>
+      <c r="H112">
+        <v>70</v>
+      </c>
+      <c r="I112">
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>0</v>
       </c>
       <c r="K112">
         <v>1</v>
@@ -5574,7 +6151,22 @@
         <v>152</v>
       </c>
       <c r="E113" t="s">
-        <v>124</v>
+        <v>123</v>
+      </c>
+      <c r="F113" t="s">
+        <v>168</v>
+      </c>
+      <c r="G113" t="s">
+        <v>162</v>
+      </c>
+      <c r="H113">
+        <v>70</v>
+      </c>
+      <c r="I113">
+        <v>0</v>
+      </c>
+      <c r="J113">
+        <v>0</v>
       </c>
       <c r="K113">
         <v>1</v>
@@ -5591,7 +6183,22 @@
         <v>152</v>
       </c>
       <c r="E114" t="s">
-        <v>125</v>
+        <v>124</v>
+      </c>
+      <c r="F114" t="s">
+        <v>168</v>
+      </c>
+      <c r="G114" t="s">
+        <v>162</v>
+      </c>
+      <c r="H114">
+        <v>70</v>
+      </c>
+      <c r="I114">
+        <v>0</v>
+      </c>
+      <c r="J114">
+        <v>0</v>
       </c>
       <c r="K114">
         <v>1</v>
@@ -5608,7 +6215,22 @@
         <v>152</v>
       </c>
       <c r="E115" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="F115" t="s">
+        <v>168</v>
+      </c>
+      <c r="G115" t="s">
+        <v>162</v>
+      </c>
+      <c r="H115">
+        <v>70</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
       </c>
       <c r="K115">
         <v>1</v>
@@ -5625,7 +6247,22 @@
         <v>152</v>
       </c>
       <c r="E116" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="F116" t="s">
+        <v>168</v>
+      </c>
+      <c r="G116" t="s">
+        <v>162</v>
+      </c>
+      <c r="H116">
+        <v>70</v>
+      </c>
+      <c r="I116">
+        <v>0</v>
+      </c>
+      <c r="J116">
+        <v>0</v>
       </c>
       <c r="K116">
         <v>1</v>
@@ -5633,16 +6270,31 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B117">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D117" t="s">
         <v>152</v>
       </c>
       <c r="E117" t="s">
-        <v>26</v>
+        <v>127</v>
+      </c>
+      <c r="F117" t="s">
+        <v>168</v>
+      </c>
+      <c r="G117" t="s">
+        <v>162</v>
+      </c>
+      <c r="H117">
+        <v>70</v>
+      </c>
+      <c r="I117">
+        <v>0</v>
+      </c>
+      <c r="J117">
+        <v>0</v>
       </c>
       <c r="K117">
         <v>1</v>
@@ -5659,7 +6311,22 @@
         <v>152</v>
       </c>
       <c r="E118" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="F118" t="s">
+        <v>168</v>
+      </c>
+      <c r="G118" t="s">
+        <v>61</v>
+      </c>
+      <c r="H118" t="s">
+        <v>162</v>
+      </c>
+      <c r="I118" t="s">
+        <v>162</v>
+      </c>
+      <c r="J118" t="s">
+        <v>162</v>
       </c>
       <c r="K118">
         <v>1</v>
@@ -5676,7 +6343,22 @@
         <v>152</v>
       </c>
       <c r="E119" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="F119" t="s">
+        <v>168</v>
+      </c>
+      <c r="G119" t="s">
+        <v>162</v>
+      </c>
+      <c r="H119" t="s">
+        <v>162</v>
+      </c>
+      <c r="I119" t="s">
+        <v>162</v>
+      </c>
+      <c r="J119" t="s">
+        <v>162</v>
       </c>
       <c r="K119">
         <v>1</v>
@@ -5693,7 +6375,22 @@
         <v>152</v>
       </c>
       <c r="E120" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="F120" t="s">
+        <v>168</v>
+      </c>
+      <c r="G120" t="s">
+        <v>162</v>
+      </c>
+      <c r="H120" t="s">
+        <v>162</v>
+      </c>
+      <c r="I120" t="s">
+        <v>162</v>
+      </c>
+      <c r="J120" t="s">
+        <v>162</v>
       </c>
       <c r="K120">
         <v>1</v>
@@ -5710,7 +6407,22 @@
         <v>152</v>
       </c>
       <c r="E121" t="s">
-        <v>128</v>
+        <v>32</v>
+      </c>
+      <c r="F121">
+        <v>0</v>
+      </c>
+      <c r="G121" t="s">
+        <v>61</v>
+      </c>
+      <c r="H121" t="s">
+        <v>162</v>
+      </c>
+      <c r="I121" t="s">
+        <v>162</v>
+      </c>
+      <c r="J121" t="s">
+        <v>162</v>
       </c>
       <c r="K121">
         <v>1</v>
@@ -5727,7 +6439,22 @@
         <v>152</v>
       </c>
       <c r="E122" t="s">
-        <v>33</v>
+        <v>128</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+      <c r="G122" t="s">
+        <v>61</v>
+      </c>
+      <c r="H122" t="s">
+        <v>162</v>
+      </c>
+      <c r="I122" t="s">
+        <v>162</v>
+      </c>
+      <c r="J122" t="s">
+        <v>162</v>
       </c>
       <c r="K122">
         <v>1</v>
@@ -5744,7 +6471,22 @@
         <v>152</v>
       </c>
       <c r="E123" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="F123" t="s">
+        <v>168</v>
+      </c>
+      <c r="G123" t="s">
+        <v>61</v>
+      </c>
+      <c r="H123" t="s">
+        <v>162</v>
+      </c>
+      <c r="I123" t="s">
+        <v>162</v>
+      </c>
+      <c r="J123" t="s">
+        <v>162</v>
       </c>
       <c r="K123">
         <v>1</v>
@@ -5761,7 +6503,22 @@
         <v>152</v>
       </c>
       <c r="E124" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="F124" t="s">
+        <v>168</v>
+      </c>
+      <c r="G124" t="s">
+        <v>162</v>
+      </c>
+      <c r="H124" t="s">
+        <v>162</v>
+      </c>
+      <c r="I124" t="s">
+        <v>162</v>
+      </c>
+      <c r="J124" t="s">
+        <v>162</v>
       </c>
       <c r="K124">
         <v>1</v>
@@ -5778,7 +6535,22 @@
         <v>152</v>
       </c>
       <c r="E125" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="F125" t="s">
+        <v>168</v>
+      </c>
+      <c r="G125" t="s">
+        <v>162</v>
+      </c>
+      <c r="H125" t="s">
+        <v>162</v>
+      </c>
+      <c r="I125" t="s">
+        <v>162</v>
+      </c>
+      <c r="J125" t="s">
+        <v>162</v>
       </c>
       <c r="K125">
         <v>1</v>
@@ -5795,7 +6567,22 @@
         <v>152</v>
       </c>
       <c r="E126" t="s">
-        <v>117</v>
+        <v>36</v>
+      </c>
+      <c r="F126" t="s">
+        <v>168</v>
+      </c>
+      <c r="G126" t="s">
+        <v>162</v>
+      </c>
+      <c r="H126" t="s">
+        <v>162</v>
+      </c>
+      <c r="I126" t="s">
+        <v>162</v>
+      </c>
+      <c r="J126" t="s">
+        <v>162</v>
       </c>
       <c r="K126">
         <v>1</v>
@@ -5812,7 +6599,22 @@
         <v>152</v>
       </c>
       <c r="E127" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="F127" t="s">
+        <v>168</v>
+      </c>
+      <c r="G127" t="s">
+        <v>162</v>
+      </c>
+      <c r="H127" t="s">
+        <v>162</v>
+      </c>
+      <c r="I127" t="s">
+        <v>162</v>
+      </c>
+      <c r="J127" t="s">
+        <v>162</v>
       </c>
       <c r="K127">
         <v>1</v>
@@ -5829,7 +6631,22 @@
         <v>152</v>
       </c>
       <c r="E128" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="F128" t="s">
+        <v>168</v>
+      </c>
+      <c r="G128" t="s">
+        <v>162</v>
+      </c>
+      <c r="H128" t="s">
+        <v>162</v>
+      </c>
+      <c r="I128" t="s">
+        <v>162</v>
+      </c>
+      <c r="J128" t="s">
+        <v>162</v>
       </c>
       <c r="K128">
         <v>1</v>
@@ -5846,7 +6663,22 @@
         <v>152</v>
       </c>
       <c r="E129" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="F129" t="s">
+        <v>168</v>
+      </c>
+      <c r="G129" t="s">
+        <v>162</v>
+      </c>
+      <c r="H129" t="s">
+        <v>162</v>
+      </c>
+      <c r="I129" t="s">
+        <v>162</v>
+      </c>
+      <c r="J129" t="s">
+        <v>162</v>
       </c>
       <c r="K129">
         <v>1</v>
@@ -5863,7 +6695,22 @@
         <v>152</v>
       </c>
       <c r="E130" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="F130" t="s">
+        <v>168</v>
+      </c>
+      <c r="G130" t="s">
+        <v>162</v>
+      </c>
+      <c r="H130" t="s">
+        <v>162</v>
+      </c>
+      <c r="I130" t="s">
+        <v>162</v>
+      </c>
+      <c r="J130" t="s">
+        <v>162</v>
       </c>
       <c r="K130">
         <v>1</v>
@@ -5880,7 +6727,22 @@
         <v>152</v>
       </c>
       <c r="E131" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="F131" t="s">
+        <v>168</v>
+      </c>
+      <c r="G131" t="s">
+        <v>162</v>
+      </c>
+      <c r="H131" t="s">
+        <v>162</v>
+      </c>
+      <c r="I131" t="s">
+        <v>162</v>
+      </c>
+      <c r="J131" t="s">
+        <v>162</v>
       </c>
       <c r="K131">
         <v>1</v>
@@ -5897,7 +6759,22 @@
         <v>152</v>
       </c>
       <c r="E132" t="s">
-        <v>123</v>
+        <v>122</v>
+      </c>
+      <c r="F132" t="s">
+        <v>168</v>
+      </c>
+      <c r="G132" t="s">
+        <v>162</v>
+      </c>
+      <c r="H132" t="s">
+        <v>162</v>
+      </c>
+      <c r="I132" t="s">
+        <v>162</v>
+      </c>
+      <c r="J132" t="s">
+        <v>162</v>
       </c>
       <c r="K132">
         <v>1</v>
@@ -5914,7 +6791,22 @@
         <v>152</v>
       </c>
       <c r="E133" t="s">
-        <v>124</v>
+        <v>123</v>
+      </c>
+      <c r="F133" t="s">
+        <v>168</v>
+      </c>
+      <c r="G133" t="s">
+        <v>162</v>
+      </c>
+      <c r="H133" t="s">
+        <v>162</v>
+      </c>
+      <c r="I133" t="s">
+        <v>162</v>
+      </c>
+      <c r="J133" t="s">
+        <v>162</v>
       </c>
       <c r="K133">
         <v>1</v>
@@ -5931,7 +6823,22 @@
         <v>152</v>
       </c>
       <c r="E134" t="s">
-        <v>125</v>
+        <v>124</v>
+      </c>
+      <c r="F134" t="s">
+        <v>168</v>
+      </c>
+      <c r="G134" t="s">
+        <v>162</v>
+      </c>
+      <c r="H134" t="s">
+        <v>162</v>
+      </c>
+      <c r="I134" t="s">
+        <v>162</v>
+      </c>
+      <c r="J134" t="s">
+        <v>162</v>
       </c>
       <c r="K134">
         <v>1</v>
@@ -5948,7 +6855,22 @@
         <v>152</v>
       </c>
       <c r="E135" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="F135" t="s">
+        <v>168</v>
+      </c>
+      <c r="G135" t="s">
+        <v>162</v>
+      </c>
+      <c r="H135" t="s">
+        <v>162</v>
+      </c>
+      <c r="I135" t="s">
+        <v>162</v>
+      </c>
+      <c r="J135" t="s">
+        <v>162</v>
       </c>
       <c r="K135">
         <v>1</v>
@@ -5965,7 +6887,22 @@
         <v>152</v>
       </c>
       <c r="E136" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="F136" t="s">
+        <v>168</v>
+      </c>
+      <c r="G136" t="s">
+        <v>162</v>
+      </c>
+      <c r="H136" t="s">
+        <v>162</v>
+      </c>
+      <c r="I136" t="s">
+        <v>162</v>
+      </c>
+      <c r="J136" t="s">
+        <v>162</v>
       </c>
       <c r="K136">
         <v>1</v>
@@ -5973,16 +6910,31 @@
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B137">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D137" t="s">
         <v>152</v>
       </c>
       <c r="E137" t="s">
-        <v>30</v>
+        <v>127</v>
+      </c>
+      <c r="F137" t="s">
+        <v>168</v>
+      </c>
+      <c r="G137" t="s">
+        <v>162</v>
+      </c>
+      <c r="H137" t="s">
+        <v>162</v>
+      </c>
+      <c r="I137" t="s">
+        <v>162</v>
+      </c>
+      <c r="J137" t="s">
+        <v>162</v>
       </c>
       <c r="K137">
         <v>1</v>
@@ -5999,10 +6951,25 @@
         <v>152</v>
       </c>
       <c r="E138" t="s">
-        <v>24</v>
-      </c>
-      <c r="K138">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="F138" t="s">
+        <v>61</v>
+      </c>
+      <c r="G138" t="s">
+        <v>61</v>
+      </c>
+      <c r="H138">
+        <v>0</v>
+      </c>
+      <c r="I138">
+        <v>0</v>
+      </c>
+      <c r="J138">
+        <v>0</v>
+      </c>
+      <c r="K138" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
@@ -6016,10 +6983,25 @@
         <v>152</v>
       </c>
       <c r="E139" t="s">
-        <v>25</v>
-      </c>
-      <c r="K139">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="F139" t="s">
+        <v>61</v>
+      </c>
+      <c r="G139" t="s">
+        <v>61</v>
+      </c>
+      <c r="H139">
+        <v>0</v>
+      </c>
+      <c r="I139">
+        <v>0</v>
+      </c>
+      <c r="J139">
+        <v>0</v>
+      </c>
+      <c r="K139" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
@@ -6033,10 +7015,25 @@
         <v>152</v>
       </c>
       <c r="E140" t="s">
-        <v>26</v>
-      </c>
-      <c r="K140">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="F140" t="s">
+        <v>61</v>
+      </c>
+      <c r="G140" t="s">
+        <v>61</v>
+      </c>
+      <c r="H140">
+        <v>0</v>
+      </c>
+      <c r="I140">
+        <v>0</v>
+      </c>
+      <c r="J140">
+        <v>0</v>
+      </c>
+      <c r="K140" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
@@ -6050,10 +7047,25 @@
         <v>152</v>
       </c>
       <c r="E141" t="s">
-        <v>27</v>
-      </c>
-      <c r="K141">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="F141" t="s">
+        <v>168</v>
+      </c>
+      <c r="G141" t="s">
+        <v>61</v>
+      </c>
+      <c r="H141">
+        <v>0</v>
+      </c>
+      <c r="I141">
+        <v>0</v>
+      </c>
+      <c r="J141">
+        <v>0</v>
+      </c>
+      <c r="K141" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
@@ -6067,10 +7079,25 @@
         <v>152</v>
       </c>
       <c r="E142" t="s">
-        <v>28</v>
-      </c>
-      <c r="K142">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="F142" t="s">
+        <v>168</v>
+      </c>
+      <c r="G142" t="s">
+        <v>162</v>
+      </c>
+      <c r="H142">
+        <v>0</v>
+      </c>
+      <c r="I142">
+        <v>0</v>
+      </c>
+      <c r="J142">
+        <v>0</v>
+      </c>
+      <c r="K142" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
@@ -6084,10 +7111,25 @@
         <v>152</v>
       </c>
       <c r="E143" t="s">
-        <v>29</v>
-      </c>
-      <c r="K143">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="F143" t="s">
+        <v>168</v>
+      </c>
+      <c r="G143" t="s">
+        <v>162</v>
+      </c>
+      <c r="H143">
+        <v>0</v>
+      </c>
+      <c r="I143">
+        <v>0</v>
+      </c>
+      <c r="J143">
+        <v>0</v>
+      </c>
+      <c r="K143" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
@@ -6101,10 +7143,25 @@
         <v>152</v>
       </c>
       <c r="E144" t="s">
-        <v>31</v>
-      </c>
-      <c r="K144">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="F144" t="s">
+        <v>168</v>
+      </c>
+      <c r="G144" t="s">
+        <v>162</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
+        <v>0</v>
+      </c>
+      <c r="J144">
+        <v>0</v>
+      </c>
+      <c r="K144" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
@@ -6118,10 +7175,25 @@
         <v>152</v>
       </c>
       <c r="E145" t="s">
-        <v>32</v>
-      </c>
-      <c r="K145">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="F145" t="s">
+        <v>61</v>
+      </c>
+      <c r="G145" t="s">
+        <v>61</v>
+      </c>
+      <c r="H145">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145">
+        <v>0</v>
+      </c>
+      <c r="K145" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
@@ -6135,10 +7207,25 @@
         <v>152</v>
       </c>
       <c r="E146" t="s">
-        <v>128</v>
-      </c>
-      <c r="K146">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="F146" t="s">
+        <v>61</v>
+      </c>
+      <c r="G146" t="s">
+        <v>61</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+      <c r="I146">
+        <v>0</v>
+      </c>
+      <c r="J146">
+        <v>0</v>
+      </c>
+      <c r="K146" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
@@ -6152,10 +7239,25 @@
         <v>152</v>
       </c>
       <c r="E147" t="s">
-        <v>33</v>
-      </c>
-      <c r="K147">
-        <v>1</v>
+        <v>128</v>
+      </c>
+      <c r="F147" t="s">
+        <v>61</v>
+      </c>
+      <c r="G147" t="s">
+        <v>61</v>
+      </c>
+      <c r="H147">
+        <v>0</v>
+      </c>
+      <c r="I147">
+        <v>0</v>
+      </c>
+      <c r="J147">
+        <v>0</v>
+      </c>
+      <c r="K147" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
@@ -6169,10 +7271,25 @@
         <v>152</v>
       </c>
       <c r="E148" t="s">
-        <v>34</v>
-      </c>
-      <c r="K148">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="F148" t="s">
+        <v>168</v>
+      </c>
+      <c r="G148" t="s">
+        <v>61</v>
+      </c>
+      <c r="H148">
+        <v>0</v>
+      </c>
+      <c r="I148">
+        <v>0</v>
+      </c>
+      <c r="J148">
+        <v>0</v>
+      </c>
+      <c r="K148" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
@@ -6186,10 +7303,25 @@
         <v>152</v>
       </c>
       <c r="E149" t="s">
-        <v>35</v>
-      </c>
-      <c r="K149">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="F149" t="s">
+        <v>168</v>
+      </c>
+      <c r="G149" t="s">
+        <v>162</v>
+      </c>
+      <c r="H149">
+        <v>0</v>
+      </c>
+      <c r="I149">
+        <v>0</v>
+      </c>
+      <c r="J149">
+        <v>0</v>
+      </c>
+      <c r="K149" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
@@ -6203,10 +7335,25 @@
         <v>152</v>
       </c>
       <c r="E150" t="s">
-        <v>36</v>
-      </c>
-      <c r="K150">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="F150" t="s">
+        <v>168</v>
+      </c>
+      <c r="G150" t="s">
+        <v>162</v>
+      </c>
+      <c r="H150">
+        <v>0</v>
+      </c>
+      <c r="I150">
+        <v>0</v>
+      </c>
+      <c r="J150">
+        <v>0</v>
+      </c>
+      <c r="K150" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
@@ -6220,10 +7367,25 @@
         <v>152</v>
       </c>
       <c r="E151" t="s">
-        <v>117</v>
-      </c>
-      <c r="K151">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="F151" t="s">
+        <v>168</v>
+      </c>
+      <c r="G151" t="s">
+        <v>162</v>
+      </c>
+      <c r="H151">
+        <v>0</v>
+      </c>
+      <c r="I151">
+        <v>0</v>
+      </c>
+      <c r="J151">
+        <v>0</v>
+      </c>
+      <c r="K151" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
@@ -6237,10 +7399,25 @@
         <v>152</v>
       </c>
       <c r="E152" t="s">
-        <v>118</v>
-      </c>
-      <c r="K152">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="F152" t="s">
+        <v>168</v>
+      </c>
+      <c r="G152" t="s">
+        <v>162</v>
+      </c>
+      <c r="H152">
+        <v>0</v>
+      </c>
+      <c r="I152">
+        <v>0</v>
+      </c>
+      <c r="J152">
+        <v>0</v>
+      </c>
+      <c r="K152" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
@@ -6254,10 +7431,25 @@
         <v>152</v>
       </c>
       <c r="E153" t="s">
-        <v>119</v>
-      </c>
-      <c r="K153">
-        <v>1</v>
+        <v>118</v>
+      </c>
+      <c r="F153" t="s">
+        <v>168</v>
+      </c>
+      <c r="G153" t="s">
+        <v>162</v>
+      </c>
+      <c r="H153">
+        <v>0</v>
+      </c>
+      <c r="I153">
+        <v>0</v>
+      </c>
+      <c r="J153">
+        <v>0</v>
+      </c>
+      <c r="K153" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
@@ -6271,10 +7463,25 @@
         <v>152</v>
       </c>
       <c r="E154" t="s">
-        <v>120</v>
-      </c>
-      <c r="K154">
-        <v>1</v>
+        <v>119</v>
+      </c>
+      <c r="F154" t="s">
+        <v>168</v>
+      </c>
+      <c r="G154" t="s">
+        <v>162</v>
+      </c>
+      <c r="H154">
+        <v>0</v>
+      </c>
+      <c r="I154">
+        <v>0</v>
+      </c>
+      <c r="J154">
+        <v>0</v>
+      </c>
+      <c r="K154" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
@@ -6288,10 +7495,25 @@
         <v>152</v>
       </c>
       <c r="E155" t="s">
-        <v>121</v>
-      </c>
-      <c r="K155">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="F155" t="s">
+        <v>168</v>
+      </c>
+      <c r="G155" t="s">
+        <v>162</v>
+      </c>
+      <c r="H155">
+        <v>0</v>
+      </c>
+      <c r="I155">
+        <v>0</v>
+      </c>
+      <c r="J155">
+        <v>0</v>
+      </c>
+      <c r="K155" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
@@ -6305,10 +7527,25 @@
         <v>152</v>
       </c>
       <c r="E156" t="s">
-        <v>122</v>
-      </c>
-      <c r="K156">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="F156" t="s">
+        <v>168</v>
+      </c>
+      <c r="G156" t="s">
+        <v>162</v>
+      </c>
+      <c r="H156">
+        <v>0</v>
+      </c>
+      <c r="I156">
+        <v>0</v>
+      </c>
+      <c r="J156">
+        <v>0</v>
+      </c>
+      <c r="K156" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
@@ -6322,10 +7559,25 @@
         <v>152</v>
       </c>
       <c r="E157" t="s">
-        <v>123</v>
-      </c>
-      <c r="K157">
-        <v>1</v>
+        <v>122</v>
+      </c>
+      <c r="F157" t="s">
+        <v>168</v>
+      </c>
+      <c r="G157" t="s">
+        <v>162</v>
+      </c>
+      <c r="H157">
+        <v>0</v>
+      </c>
+      <c r="I157">
+        <v>0</v>
+      </c>
+      <c r="J157">
+        <v>0</v>
+      </c>
+      <c r="K157" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
@@ -6339,10 +7591,25 @@
         <v>152</v>
       </c>
       <c r="E158" t="s">
-        <v>124</v>
-      </c>
-      <c r="K158">
-        <v>1</v>
+        <v>123</v>
+      </c>
+      <c r="F158" t="s">
+        <v>168</v>
+      </c>
+      <c r="G158" t="s">
+        <v>162</v>
+      </c>
+      <c r="H158">
+        <v>0</v>
+      </c>
+      <c r="I158">
+        <v>0</v>
+      </c>
+      <c r="J158">
+        <v>0</v>
+      </c>
+      <c r="K158" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.25">
@@ -6356,10 +7623,25 @@
         <v>152</v>
       </c>
       <c r="E159" t="s">
-        <v>125</v>
-      </c>
-      <c r="K159">
-        <v>1</v>
+        <v>124</v>
+      </c>
+      <c r="F159" t="s">
+        <v>168</v>
+      </c>
+      <c r="G159" t="s">
+        <v>162</v>
+      </c>
+      <c r="H159">
+        <v>0</v>
+      </c>
+      <c r="I159">
+        <v>0</v>
+      </c>
+      <c r="J159">
+        <v>0</v>
+      </c>
+      <c r="K159" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.25">
@@ -6373,10 +7655,25 @@
         <v>152</v>
       </c>
       <c r="E160" t="s">
-        <v>126</v>
-      </c>
-      <c r="K160">
-        <v>1</v>
+        <v>125</v>
+      </c>
+      <c r="F160" t="s">
+        <v>168</v>
+      </c>
+      <c r="G160" t="s">
+        <v>162</v>
+      </c>
+      <c r="H160">
+        <v>0</v>
+      </c>
+      <c r="I160">
+        <v>0</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+      <c r="K160" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
@@ -6390,10 +7687,25 @@
         <v>152</v>
       </c>
       <c r="E161" t="s">
-        <v>127</v>
-      </c>
-      <c r="K161">
-        <v>1</v>
+        <v>126</v>
+      </c>
+      <c r="F161" t="s">
+        <v>168</v>
+      </c>
+      <c r="G161" t="s">
+        <v>162</v>
+      </c>
+      <c r="H161">
+        <v>0</v>
+      </c>
+      <c r="I161">
+        <v>0</v>
+      </c>
+      <c r="J161">
+        <v>0</v>
+      </c>
+      <c r="K161" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
@@ -6407,10 +7719,25 @@
         <v>152</v>
       </c>
       <c r="E162" t="s">
-        <v>37</v>
-      </c>
-      <c r="K162">
-        <v>1</v>
+        <v>127</v>
+      </c>
+      <c r="F162" t="s">
+        <v>168</v>
+      </c>
+      <c r="G162" t="s">
+        <v>162</v>
+      </c>
+      <c r="H162">
+        <v>0</v>
+      </c>
+      <c r="I162">
+        <v>0</v>
+      </c>
+      <c r="J162">
+        <v>0</v>
+      </c>
+      <c r="K162" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
@@ -6424,33 +7751,57 @@
         <v>152</v>
       </c>
       <c r="E163" t="s">
-        <v>62</v>
-      </c>
-      <c r="I163" t="s">
-        <v>61</v>
-      </c>
-      <c r="J163" t="s">
-        <v>61</v>
-      </c>
-      <c r="K163">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="F163" t="s">
+        <v>61</v>
+      </c>
+      <c r="G163" t="s">
+        <v>61</v>
+      </c>
+      <c r="H163">
+        <v>0</v>
+      </c>
+      <c r="I163">
+        <v>0</v>
+      </c>
+      <c r="J163">
+        <v>0</v>
+      </c>
+      <c r="K163" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="B164">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D164" t="s">
         <v>152</v>
       </c>
       <c r="E164" t="s">
-        <v>31</v>
-      </c>
-      <c r="K164">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="F164" t="s">
+        <v>61</v>
+      </c>
+      <c r="G164" t="s">
+        <v>169</v>
+      </c>
+      <c r="H164" t="s">
+        <v>61</v>
+      </c>
+      <c r="I164" t="s">
+        <v>61</v>
+      </c>
+      <c r="J164" t="s">
+        <v>61</v>
+      </c>
+      <c r="K164" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.25">
@@ -6464,7 +7815,22 @@
         <v>152</v>
       </c>
       <c r="E165" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="F165" t="s">
+        <v>61</v>
+      </c>
+      <c r="G165" t="s">
+        <v>61</v>
+      </c>
+      <c r="H165">
+        <v>0</v>
+      </c>
+      <c r="I165">
+        <v>0</v>
+      </c>
+      <c r="J165">
+        <v>0</v>
       </c>
       <c r="K165">
         <v>1</v>
@@ -6481,7 +7847,22 @@
         <v>152</v>
       </c>
       <c r="E166" t="s">
-        <v>128</v>
+        <v>32</v>
+      </c>
+      <c r="F166" t="s">
+        <v>61</v>
+      </c>
+      <c r="G166" t="s">
+        <v>61</v>
+      </c>
+      <c r="H166">
+        <v>0</v>
+      </c>
+      <c r="I166">
+        <v>0</v>
+      </c>
+      <c r="J166">
+        <v>0</v>
       </c>
       <c r="K166">
         <v>1</v>
@@ -6498,7 +7879,22 @@
         <v>152</v>
       </c>
       <c r="E167" t="s">
-        <v>33</v>
+        <v>128</v>
+      </c>
+      <c r="F167" t="s">
+        <v>61</v>
+      </c>
+      <c r="G167" t="s">
+        <v>61</v>
+      </c>
+      <c r="H167">
+        <v>0</v>
+      </c>
+      <c r="I167">
+        <v>0</v>
+      </c>
+      <c r="J167">
+        <v>0</v>
       </c>
       <c r="K167">
         <v>1</v>
@@ -6515,7 +7911,22 @@
         <v>152</v>
       </c>
       <c r="E168" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="F168" t="s">
+        <v>168</v>
+      </c>
+      <c r="G168" t="s">
+        <v>61</v>
+      </c>
+      <c r="H168">
+        <v>0</v>
+      </c>
+      <c r="I168">
+        <v>0</v>
+      </c>
+      <c r="J168">
+        <v>0</v>
       </c>
       <c r="K168">
         <v>1</v>
@@ -6532,7 +7943,22 @@
         <v>152</v>
       </c>
       <c r="E169" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="F169" t="s">
+        <v>168</v>
+      </c>
+      <c r="G169" t="s">
+        <v>162</v>
+      </c>
+      <c r="H169">
+        <v>0</v>
+      </c>
+      <c r="I169">
+        <v>0</v>
+      </c>
+      <c r="J169">
+        <v>0</v>
       </c>
       <c r="K169">
         <v>1</v>
@@ -6549,7 +7975,22 @@
         <v>152</v>
       </c>
       <c r="E170" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="F170" t="s">
+        <v>168</v>
+      </c>
+      <c r="G170" t="s">
+        <v>162</v>
+      </c>
+      <c r="H170">
+        <v>0</v>
+      </c>
+      <c r="I170">
+        <v>0</v>
+      </c>
+      <c r="J170">
+        <v>0</v>
       </c>
       <c r="K170">
         <v>1</v>
@@ -6566,7 +8007,22 @@
         <v>152</v>
       </c>
       <c r="E171" t="s">
-        <v>123</v>
+        <v>36</v>
+      </c>
+      <c r="F171" t="s">
+        <v>168</v>
+      </c>
+      <c r="G171" t="s">
+        <v>162</v>
+      </c>
+      <c r="H171">
+        <v>0</v>
+      </c>
+      <c r="I171">
+        <v>0</v>
+      </c>
+      <c r="J171">
+        <v>0</v>
       </c>
       <c r="K171">
         <v>1</v>
@@ -6583,7 +8039,22 @@
         <v>152</v>
       </c>
       <c r="E172" t="s">
-        <v>124</v>
+        <v>123</v>
+      </c>
+      <c r="F172" t="s">
+        <v>168</v>
+      </c>
+      <c r="G172" t="s">
+        <v>162</v>
+      </c>
+      <c r="H172">
+        <v>0</v>
+      </c>
+      <c r="I172">
+        <v>0</v>
+      </c>
+      <c r="J172">
+        <v>0</v>
       </c>
       <c r="K172">
         <v>1</v>
@@ -6600,7 +8071,22 @@
         <v>152</v>
       </c>
       <c r="E173" t="s">
-        <v>125</v>
+        <v>124</v>
+      </c>
+      <c r="F173" t="s">
+        <v>168</v>
+      </c>
+      <c r="G173" t="s">
+        <v>162</v>
+      </c>
+      <c r="H173">
+        <v>0</v>
+      </c>
+      <c r="I173">
+        <v>0</v>
+      </c>
+      <c r="J173">
+        <v>0</v>
       </c>
       <c r="K173">
         <v>1</v>
@@ -6617,7 +8103,22 @@
         <v>152</v>
       </c>
       <c r="E174" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="F174" t="s">
+        <v>168</v>
+      </c>
+      <c r="G174" t="s">
+        <v>162</v>
+      </c>
+      <c r="H174">
+        <v>0</v>
+      </c>
+      <c r="I174">
+        <v>0</v>
+      </c>
+      <c r="J174">
+        <v>0</v>
       </c>
       <c r="K174">
         <v>1</v>
@@ -6634,7 +8135,22 @@
         <v>152</v>
       </c>
       <c r="E175" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="F175" t="s">
+        <v>168</v>
+      </c>
+      <c r="G175" t="s">
+        <v>162</v>
+      </c>
+      <c r="H175">
+        <v>0</v>
+      </c>
+      <c r="I175">
+        <v>0</v>
+      </c>
+      <c r="J175">
+        <v>0</v>
       </c>
       <c r="K175">
         <v>1</v>
@@ -6651,7 +8167,22 @@
         <v>152</v>
       </c>
       <c r="E176" t="s">
-        <v>37</v>
+        <v>127</v>
+      </c>
+      <c r="F176" t="s">
+        <v>168</v>
+      </c>
+      <c r="G176" t="s">
+        <v>162</v>
+      </c>
+      <c r="H176">
+        <v>0</v>
+      </c>
+      <c r="I176">
+        <v>0</v>
+      </c>
+      <c r="J176">
+        <v>0</v>
       </c>
       <c r="K176">
         <v>1</v>
@@ -6659,22 +8190,31 @@
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="B177">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D177" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E177" t="s">
-        <v>62</v>
-      </c>
-      <c r="I177" t="s">
-        <v>61</v>
-      </c>
-      <c r="J177" t="s">
-        <v>61</v>
+        <v>37</v>
+      </c>
+      <c r="F177" t="s">
+        <v>168</v>
+      </c>
+      <c r="G177" t="s">
+        <v>162</v>
+      </c>
+      <c r="H177">
+        <v>0</v>
+      </c>
+      <c r="I177">
+        <v>0</v>
+      </c>
+      <c r="J177">
+        <v>0</v>
       </c>
       <c r="K177">
         <v>1</v>
@@ -6682,34 +8222,94 @@
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="B178">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D178" t="s">
         <v>150</v>
       </c>
       <c r="E178" t="s">
+        <v>133</v>
+      </c>
+      <c r="F178" t="s">
+        <v>61</v>
+      </c>
+      <c r="G178" t="s">
+        <v>165</v>
+      </c>
+      <c r="H178" t="s">
+        <v>61</v>
+      </c>
+      <c r="I178" t="s">
+        <v>61</v>
+      </c>
+      <c r="J178" t="s">
+        <v>61</v>
+      </c>
+      <c r="K178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B179">
+        <v>27</v>
+      </c>
+      <c r="D179" t="s">
+        <v>150</v>
+      </c>
+      <c r="E179" t="s">
         <v>130</v>
       </c>
-      <c r="F178">
-        <v>0</v>
-      </c>
-      <c r="G178" t="s">
+      <c r="F179">
+        <v>0</v>
+      </c>
+      <c r="G179" t="s">
         <v>131</v>
       </c>
-      <c r="I178" t="s">
-        <v>61</v>
-      </c>
-      <c r="J178" t="s">
-        <v>61</v>
-      </c>
-      <c r="K178">
+      <c r="H179" t="s">
+        <v>61</v>
+      </c>
+      <c r="I179" t="s">
+        <v>61</v>
+      </c>
+      <c r="J179" t="s">
+        <v>61</v>
+      </c>
+      <c r="K179">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F1:K9 F11:K90">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(F1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:K9 F11:K179">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(F1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:G10 I10:K10">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(F10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(H10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(H10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
i think its mostly done. i need a new mode function. about to copy the logic from primary to relative so pushing now in case i mess that up
</commit_message>
<xml_diff>
--- a/test_constraints.xlsx
+++ b/test_constraints.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HumeD\PycharmProjects\Data_Profile_Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC32AA9-22DC-43C5-9F8E-319A0F333FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40EF289-5A1E-4783-8428-AEB43045019A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{D2E9D144-5D6F-4AC1-9DA3-D4FF634D9598}"/>
   </bookViews>
   <sheets>
     <sheet name="Constraint Set Definitions" sheetId="1" r:id="rId1"/>
     <sheet name="Constraint Definitions" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="Data Set Definitions" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Data Set Definitions" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Constraint Definitions'!$D$1:$D$400</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2859" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2860" uniqueCount="198">
   <si>
     <t>Constraint_Set_Name</t>
   </si>
@@ -691,7 +692,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1450,8 +1458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E86614-3B97-43D1-B6C4-36CEB2305CDA}">
   <dimension ref="A1:K400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D167" workbookViewId="0">
-      <selection activeCell="G180" sqref="G180"/>
+    <sheetView tabSelected="1" topLeftCell="D82" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3731,7 +3739,7 @@
         <v>144</v>
       </c>
       <c r="H65">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I65">
         <v>100</v>
@@ -3766,7 +3774,7 @@
         <v>144</v>
       </c>
       <c r="H66">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I66">
         <v>0</v>
@@ -3801,7 +3809,7 @@
         <v>144</v>
       </c>
       <c r="H67">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I67">
         <v>1</v>
@@ -4781,7 +4789,7 @@
         <v>144</v>
       </c>
       <c r="H95">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I95">
         <v>100</v>
@@ -4816,7 +4824,7 @@
         <v>144</v>
       </c>
       <c r="H96">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I96">
         <v>0</v>
@@ -4851,7 +4859,7 @@
         <v>144</v>
       </c>
       <c r="H97">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I97">
         <v>1</v>
@@ -5306,7 +5314,7 @@
         <v>144</v>
       </c>
       <c r="H110">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I110">
         <v>100</v>
@@ -5341,7 +5349,7 @@
         <v>144</v>
       </c>
       <c r="H111">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I111">
         <v>0</v>
@@ -5376,7 +5384,7 @@
         <v>144</v>
       </c>
       <c r="H112">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I112">
         <v>1</v>
@@ -5831,7 +5839,7 @@
         <v>144</v>
       </c>
       <c r="H125">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I125">
         <v>100</v>
@@ -5866,7 +5874,7 @@
         <v>144</v>
       </c>
       <c r="H126">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I126">
         <v>0</v>
@@ -5901,7 +5909,7 @@
         <v>144</v>
       </c>
       <c r="H127">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I127">
         <v>1</v>
@@ -6356,7 +6364,7 @@
         <v>144</v>
       </c>
       <c r="H140">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I140">
         <v>100</v>
@@ -6391,7 +6399,7 @@
         <v>144</v>
       </c>
       <c r="H141">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I141">
         <v>0</v>
@@ -6426,7 +6434,7 @@
         <v>144</v>
       </c>
       <c r="H142">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I142">
         <v>1</v>
@@ -6881,7 +6889,7 @@
         <v>144</v>
       </c>
       <c r="H155">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I155">
         <v>100</v>
@@ -6916,7 +6924,7 @@
         <v>144</v>
       </c>
       <c r="H156">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I156">
         <v>0</v>
@@ -6951,7 +6959,7 @@
         <v>144</v>
       </c>
       <c r="H157">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I157">
         <v>1</v>
@@ -15469,153 +15477,153 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C186:K186 A1:K1 J187:K187 K188:K190 C394:C398 C400 C391:F391 G392:G393 A2:B400 C2:K182 C187:H188 C190:F190 C189:G189 H189:H190 C191:K390">
-    <cfRule type="containsBlanks" dxfId="29" priority="31">
+  <conditionalFormatting sqref="C186:K186 A1:K1 J187:K187 K188:K190 C394:C398 C400 C391:F391 G392:G393 C187:H188 C190:F190 C189:G189 H189:H190 C191:K390 A2:B400 C2:K182">
+    <cfRule type="containsBlanks" dxfId="30" priority="31">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C183:C185">
-    <cfRule type="containsBlanks" dxfId="28" priority="30">
+    <cfRule type="containsBlanks" dxfId="29" priority="30">
       <formula>LEN(TRIM(C183))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="containsBlanks" dxfId="27" priority="29">
+    <cfRule type="containsBlanks" dxfId="28" priority="29">
       <formula>LEN(TRIM(D183))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D184">
-    <cfRule type="containsBlanks" dxfId="26" priority="28">
+    <cfRule type="containsBlanks" dxfId="27" priority="28">
       <formula>LEN(TRIM(D184))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D185">
-    <cfRule type="containsBlanks" dxfId="25" priority="27">
+    <cfRule type="containsBlanks" dxfId="26" priority="27">
       <formula>LEN(TRIM(D185))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E183">
-    <cfRule type="containsBlanks" dxfId="24" priority="26">
+    <cfRule type="containsBlanks" dxfId="25" priority="26">
       <formula>LEN(TRIM(E183))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E184">
-    <cfRule type="containsBlanks" dxfId="23" priority="25">
+    <cfRule type="containsBlanks" dxfId="24" priority="25">
       <formula>LEN(TRIM(E184))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E185">
-    <cfRule type="containsBlanks" dxfId="22" priority="24">
+    <cfRule type="containsBlanks" dxfId="23" priority="24">
       <formula>LEN(TRIM(E185))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F183:K183">
-    <cfRule type="containsBlanks" dxfId="21" priority="23">
+    <cfRule type="containsBlanks" dxfId="22" priority="23">
       <formula>LEN(TRIM(F183))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F184:K184">
-    <cfRule type="containsBlanks" dxfId="20" priority="22">
+    <cfRule type="containsBlanks" dxfId="21" priority="22">
       <formula>LEN(TRIM(F184))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F185:K185">
-    <cfRule type="containsBlanks" dxfId="19" priority="21">
+    <cfRule type="containsBlanks" dxfId="20" priority="21">
       <formula>LEN(TRIM(F185))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I187">
-    <cfRule type="containsBlanks" dxfId="18" priority="20">
+    <cfRule type="containsBlanks" dxfId="19" priority="20">
       <formula>LEN(TRIM(I187))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I188">
-    <cfRule type="containsBlanks" dxfId="17" priority="19">
+    <cfRule type="containsBlanks" dxfId="18" priority="19">
       <formula>LEN(TRIM(I188))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J188">
-    <cfRule type="containsBlanks" dxfId="16" priority="18">
+    <cfRule type="containsBlanks" dxfId="17" priority="18">
       <formula>LEN(TRIM(J188))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J189">
-    <cfRule type="containsBlanks" dxfId="15" priority="17">
+    <cfRule type="containsBlanks" dxfId="16" priority="17">
       <formula>LEN(TRIM(J189))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I189">
-    <cfRule type="containsBlanks" dxfId="14" priority="16">
+    <cfRule type="containsBlanks" dxfId="15" priority="16">
       <formula>LEN(TRIM(I189))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I190">
-    <cfRule type="containsBlanks" dxfId="13" priority="15">
+    <cfRule type="containsBlanks" dxfId="14" priority="15">
       <formula>LEN(TRIM(I190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J190">
-    <cfRule type="containsBlanks" dxfId="12" priority="14">
+    <cfRule type="containsBlanks" dxfId="13" priority="14">
       <formula>LEN(TRIM(J190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C392">
-    <cfRule type="containsBlanks" dxfId="11" priority="13">
+    <cfRule type="containsBlanks" dxfId="12" priority="13">
       <formula>LEN(TRIM(C392))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C393">
-    <cfRule type="containsBlanks" dxfId="10" priority="12">
+    <cfRule type="containsBlanks" dxfId="11" priority="12">
       <formula>LEN(TRIM(C393))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C399">
-    <cfRule type="containsBlanks" dxfId="9" priority="10">
+    <cfRule type="containsBlanks" dxfId="10" priority="10">
       <formula>LEN(TRIM(C399))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D392:D398 D400">
-    <cfRule type="containsBlanks" dxfId="8" priority="9">
+    <cfRule type="containsBlanks" dxfId="9" priority="9">
       <formula>LEN(TRIM(D392))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D399">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
+    <cfRule type="containsBlanks" dxfId="8" priority="8">
       <formula>LEN(TRIM(D399))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E392:E400">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="7" priority="7">
       <formula>LEN(TRIM(E392))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F392:F400">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="6" priority="6">
       <formula>LEN(TRIM(F392))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G394:G400">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(G394))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G391">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="4" priority="4">
       <formula>LEN(TRIM(G391))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H393">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(H393))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I391:K400">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(I391))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(G190))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15625,6 +15633,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38F7402-8428-4FC7-B0C9-15F7BD0E8F19}">
+  <dimension ref="I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(I17))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ECEEAC-9EEA-413B-A85A-FBAD48F16B14}">
   <dimension ref="J8:J9"/>
   <sheetViews>
@@ -15647,7 +15680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15001D91-9CB8-4DAB-A1A3-2C399064AEE1}">
   <dimension ref="A1:C3"/>
   <sheetViews>

</xml_diff>

<commit_message>
all tests passing, test coverage at 89%. I think that adding some new input data for test cases will reveal a few more semantic errors, but most of the remaining work is inputting the right test cases.
</commit_message>
<xml_diff>
--- a/test_constraints.xlsx
+++ b/test_constraints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HumeD\PycharmProjects\Data_Profile_Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511BF8F4-9A64-4899-ACA5-3D56699C5736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D15C220-2A0C-42EA-BB0D-2F97B929D50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{D2E9D144-5D6F-4AC1-9DA3-D4FF634D9598}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2955" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3048" uniqueCount="524">
   <si>
     <t>Constraint_Set_Name</t>
   </si>
@@ -1538,6 +1538,81 @@
   </si>
   <si>
     <t>C-4Pass: DCP EM Sum ( 1 &lt;= 1 &lt;= 1 )</t>
+  </si>
+  <si>
+    <t>Absolute Column Min</t>
+  </si>
+  <si>
+    <t>Relative Column Min</t>
+  </si>
+  <si>
+    <t>Absolute Column Mean</t>
+  </si>
+  <si>
+    <t>Relative Column Mean</t>
+  </si>
+  <si>
+    <t>Absolute Column Median</t>
+  </si>
+  <si>
+    <t>Relative Column Median</t>
+  </si>
+  <si>
+    <t>Absolute Column Mode</t>
+  </si>
+  <si>
+    <t>Relative Column Mode</t>
+  </si>
+  <si>
+    <t>Absolute Column Max</t>
+  </si>
+  <si>
+    <t>Relative Column Max</t>
+  </si>
+  <si>
+    <t>C408PASS: Absolute Column Min</t>
+  </si>
+  <si>
+    <t>C410PASS: Absolute Column Mean</t>
+  </si>
+  <si>
+    <t>C412PASS: Absolute Column Median</t>
+  </si>
+  <si>
+    <t>C414PASS: Absolute Column Mode</t>
+  </si>
+  <si>
+    <t>C416PASS: Absolute Column Max</t>
+  </si>
+  <si>
+    <t>C417PASS: Relative Column Max Ratio</t>
+  </si>
+  <si>
+    <t>C415PASS: Relative Column Mode Ratio</t>
+  </si>
+  <si>
+    <t>C413PASS: Relative Column Median Ratio</t>
+  </si>
+  <si>
+    <t>C411PASS: Relative Column Mean Ratio</t>
+  </si>
+  <si>
+    <t>C409PASS: Relative Column Min Ratio</t>
+  </si>
+  <si>
+    <t>C418PASS: Absolute Column Data Type</t>
+  </si>
+  <si>
+    <t>C419PASS: Relative Column Data Type</t>
+  </si>
+  <si>
+    <t>C420PASS: Absolute Column Name</t>
+  </si>
+  <si>
+    <t>C421PASS: Relative Column Name</t>
+  </si>
+  <si>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -1601,7 +1676,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="85">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2708,10 +2818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E86614-3B97-43D1-B6C4-36CEB2305CDA}">
-  <dimension ref="A1:K415"/>
+  <dimension ref="A1:K429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2887,6 +2997,12 @@
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
       <c r="I6" t="s">
         <v>21</v>
       </c>
@@ -2958,10 +3074,10 @@
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>523</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>523</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -13283,10 +13399,10 @@
         <v>4</v>
       </c>
       <c r="I303">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J303">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K303">
         <v>1</v>
@@ -14333,10 +14449,10 @@
         <v>4</v>
       </c>
       <c r="I333">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J333">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K333">
         <v>1</v>
@@ -14858,10 +14974,10 @@
         <v>4</v>
       </c>
       <c r="I348">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J348">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K348">
         <v>1</v>
@@ -15383,10 +15499,10 @@
         <v>4</v>
       </c>
       <c r="I363">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J363">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K363">
         <v>1</v>
@@ -17209,389 +17325,899 @@
         <v>21</v>
       </c>
       <c r="K415">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A416" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B416">
+        <v>1</v>
+      </c>
+      <c r="C416" t="s">
+        <v>509</v>
+      </c>
+      <c r="D416" t="s">
+        <v>43</v>
+      </c>
+      <c r="E416" t="s">
+        <v>499</v>
+      </c>
+      <c r="F416" t="s">
+        <v>21</v>
+      </c>
+      <c r="G416" t="s">
+        <v>21</v>
+      </c>
+      <c r="H416">
+        <v>0</v>
+      </c>
+      <c r="I416">
+        <v>1</v>
+      </c>
+      <c r="J416">
+        <v>1</v>
+      </c>
+      <c r="K416">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A417" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B417">
+        <v>1</v>
+      </c>
+      <c r="C417" t="s">
+        <v>518</v>
+      </c>
+      <c r="D417" t="s">
+        <v>43</v>
+      </c>
+      <c r="E417" t="s">
+        <v>500</v>
+      </c>
+      <c r="F417" t="s">
+        <v>21</v>
+      </c>
+      <c r="G417" t="s">
+        <v>21</v>
+      </c>
+      <c r="H417">
+        <v>0</v>
+      </c>
+      <c r="I417">
+        <v>1</v>
+      </c>
+      <c r="J417">
+        <v>1</v>
+      </c>
+      <c r="K417">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A418" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B418">
+        <v>1</v>
+      </c>
+      <c r="C418" t="s">
+        <v>510</v>
+      </c>
+      <c r="D418" t="s">
+        <v>43</v>
+      </c>
+      <c r="E418" t="s">
+        <v>501</v>
+      </c>
+      <c r="F418" t="s">
+        <v>21</v>
+      </c>
+      <c r="G418" t="s">
+        <v>21</v>
+      </c>
+      <c r="H418">
+        <v>4</v>
+      </c>
+      <c r="I418">
+        <v>5</v>
+      </c>
+      <c r="J418">
+        <v>5</v>
+      </c>
+      <c r="K418">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A419" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B419">
+        <v>1</v>
+      </c>
+      <c r="C419" t="s">
+        <v>517</v>
+      </c>
+      <c r="D419" t="s">
+        <v>43</v>
+      </c>
+      <c r="E419" t="s">
+        <v>502</v>
+      </c>
+      <c r="F419" t="s">
+        <v>21</v>
+      </c>
+      <c r="G419" t="s">
+        <v>21</v>
+      </c>
+      <c r="H419">
+        <v>4</v>
+      </c>
+      <c r="I419">
+        <v>1</v>
+      </c>
+      <c r="J419">
+        <v>1</v>
+      </c>
+      <c r="K419">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A420" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B420">
+        <v>1</v>
+      </c>
+      <c r="C420" t="s">
+        <v>511</v>
+      </c>
+      <c r="D420" t="s">
+        <v>43</v>
+      </c>
+      <c r="E420" t="s">
+        <v>503</v>
+      </c>
+      <c r="F420" t="s">
+        <v>21</v>
+      </c>
+      <c r="G420" t="s">
+        <v>21</v>
+      </c>
+      <c r="H420">
+        <v>4</v>
+      </c>
+      <c r="I420">
+        <v>5</v>
+      </c>
+      <c r="J420">
+        <v>5</v>
+      </c>
+      <c r="K420">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A421" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B421">
+        <v>1</v>
+      </c>
+      <c r="C421" t="s">
+        <v>516</v>
+      </c>
+      <c r="D421" t="s">
+        <v>43</v>
+      </c>
+      <c r="E421" t="s">
+        <v>504</v>
+      </c>
+      <c r="F421" t="s">
+        <v>21</v>
+      </c>
+      <c r="G421" t="s">
+        <v>21</v>
+      </c>
+      <c r="H421">
+        <v>4</v>
+      </c>
+      <c r="I421">
+        <v>1</v>
+      </c>
+      <c r="J421">
+        <v>1</v>
+      </c>
+      <c r="K421">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A422" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B422">
+        <v>1</v>
+      </c>
+      <c r="C422" t="s">
+        <v>512</v>
+      </c>
+      <c r="D422" t="s">
+        <v>43</v>
+      </c>
+      <c r="E422" t="s">
+        <v>505</v>
+      </c>
+      <c r="F422" t="s">
+        <v>21</v>
+      </c>
+      <c r="G422" t="s">
+        <v>21</v>
+      </c>
+      <c r="H422">
+        <v>6</v>
+      </c>
+      <c r="I422">
+        <v>10</v>
+      </c>
+      <c r="J422">
+        <v>10</v>
+      </c>
+      <c r="K422">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A423" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B423">
+        <v>1</v>
+      </c>
+      <c r="C423" t="s">
+        <v>515</v>
+      </c>
+      <c r="D423" t="s">
+        <v>43</v>
+      </c>
+      <c r="E423" t="s">
+        <v>506</v>
+      </c>
+      <c r="F423" t="s">
+        <v>21</v>
+      </c>
+      <c r="G423" t="s">
+        <v>21</v>
+      </c>
+      <c r="H423">
+        <v>6</v>
+      </c>
+      <c r="I423">
+        <v>1</v>
+      </c>
+      <c r="J423">
+        <v>1</v>
+      </c>
+      <c r="K423">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A424" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B424">
+        <v>1</v>
+      </c>
+      <c r="C424" t="s">
+        <v>513</v>
+      </c>
+      <c r="D424" t="s">
+        <v>43</v>
+      </c>
+      <c r="E424" t="s">
+        <v>507</v>
+      </c>
+      <c r="F424" t="s">
+        <v>21</v>
+      </c>
+      <c r="G424" t="s">
+        <v>21</v>
+      </c>
+      <c r="H424">
+        <v>6</v>
+      </c>
+      <c r="I424">
+        <v>10</v>
+      </c>
+      <c r="J424">
+        <v>10</v>
+      </c>
+      <c r="K424">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A425" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B425">
+        <v>1</v>
+      </c>
+      <c r="C425" t="s">
+        <v>514</v>
+      </c>
+      <c r="D425" t="s">
+        <v>43</v>
+      </c>
+      <c r="E425" t="s">
+        <v>508</v>
+      </c>
+      <c r="F425" t="s">
+        <v>21</v>
+      </c>
+      <c r="G425" t="s">
+        <v>21</v>
+      </c>
+      <c r="H425">
+        <v>6</v>
+      </c>
+      <c r="I425">
+        <v>1</v>
+      </c>
+      <c r="J425">
+        <v>1</v>
+      </c>
+      <c r="K425">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A426" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B426">
+        <v>1</v>
+      </c>
+      <c r="C426" t="s">
+        <v>519</v>
+      </c>
+      <c r="D426" t="s">
+        <v>43</v>
+      </c>
+      <c r="E426" t="s">
+        <v>59</v>
+      </c>
+      <c r="F426" t="s">
+        <v>21</v>
+      </c>
+      <c r="G426" t="s">
+        <v>50</v>
+      </c>
+      <c r="H426">
+        <v>0</v>
+      </c>
+      <c r="I426" t="s">
+        <v>21</v>
+      </c>
+      <c r="J426" t="s">
+        <v>21</v>
+      </c>
+      <c r="K426">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A427" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B427">
+        <v>1</v>
+      </c>
+      <c r="C427" t="s">
+        <v>520</v>
+      </c>
+      <c r="D427" t="s">
+        <v>43</v>
+      </c>
+      <c r="E427" t="s">
+        <v>65</v>
+      </c>
+      <c r="F427" t="s">
+        <v>21</v>
+      </c>
+      <c r="G427" t="s">
+        <v>21</v>
+      </c>
+      <c r="H427">
+        <v>0</v>
+      </c>
+      <c r="I427" t="s">
+        <v>21</v>
+      </c>
+      <c r="J427" t="s">
+        <v>21</v>
+      </c>
+      <c r="K427">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A428" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B428">
+        <v>1</v>
+      </c>
+      <c r="C428" t="s">
+        <v>521</v>
+      </c>
+      <c r="D428" t="s">
+        <v>43</v>
+      </c>
+      <c r="E428" t="s">
+        <v>60</v>
+      </c>
+      <c r="F428" t="s">
+        <v>21</v>
+      </c>
+      <c r="G428" t="s">
+        <v>41</v>
+      </c>
+      <c r="H428">
+        <v>0</v>
+      </c>
+      <c r="I428" t="s">
+        <v>21</v>
+      </c>
+      <c r="J428" t="s">
+        <v>21</v>
+      </c>
+      <c r="K428">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A429" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B429">
+        <v>1</v>
+      </c>
+      <c r="C429" t="s">
+        <v>522</v>
+      </c>
+      <c r="D429" t="s">
+        <v>43</v>
+      </c>
+      <c r="E429" t="s">
+        <v>67</v>
+      </c>
+      <c r="F429" t="s">
+        <v>21</v>
+      </c>
+      <c r="G429" t="s">
+        <v>21</v>
+      </c>
+      <c r="H429">
+        <v>0</v>
+      </c>
+      <c r="I429" t="s">
+        <v>21</v>
+      </c>
+      <c r="J429" t="s">
+        <v>21</v>
+      </c>
+      <c r="K429">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C193:K193 J194:K194 K195:K197 C401:C405 C407 C398:F398 G399:G400 C194:H195 C197:F197 C196:G196 H196:H197 C9:K189 A9:B407 C198:K397 A1:K2 A7:E7">
-    <cfRule type="containsBlanks" dxfId="79" priority="77">
+    <cfRule type="containsBlanks" dxfId="84" priority="82">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C190:C192">
-    <cfRule type="containsBlanks" dxfId="78" priority="76">
+    <cfRule type="containsBlanks" dxfId="83" priority="81">
       <formula>LEN(TRIM(C190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D190">
-    <cfRule type="containsBlanks" dxfId="77" priority="75">
+    <cfRule type="containsBlanks" dxfId="82" priority="80">
       <formula>LEN(TRIM(D190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="containsBlanks" dxfId="76" priority="74">
+    <cfRule type="containsBlanks" dxfId="81" priority="79">
       <formula>LEN(TRIM(D191))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D192">
-    <cfRule type="containsBlanks" dxfId="75" priority="73">
+    <cfRule type="containsBlanks" dxfId="80" priority="78">
       <formula>LEN(TRIM(D192))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E190">
-    <cfRule type="containsBlanks" dxfId="74" priority="72">
+    <cfRule type="containsBlanks" dxfId="79" priority="77">
       <formula>LEN(TRIM(E190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E191">
-    <cfRule type="containsBlanks" dxfId="73" priority="71">
+    <cfRule type="containsBlanks" dxfId="78" priority="76">
       <formula>LEN(TRIM(E191))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E192">
-    <cfRule type="containsBlanks" dxfId="72" priority="70">
+    <cfRule type="containsBlanks" dxfId="77" priority="75">
       <formula>LEN(TRIM(E192))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F190:K190">
-    <cfRule type="containsBlanks" dxfId="71" priority="69">
+    <cfRule type="containsBlanks" dxfId="76" priority="74">
       <formula>LEN(TRIM(F190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F191:K191">
-    <cfRule type="containsBlanks" dxfId="70" priority="68">
+    <cfRule type="containsBlanks" dxfId="75" priority="73">
       <formula>LEN(TRIM(F191))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F192:K192">
-    <cfRule type="containsBlanks" dxfId="69" priority="67">
+    <cfRule type="containsBlanks" dxfId="74" priority="72">
       <formula>LEN(TRIM(F192))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I194">
-    <cfRule type="containsBlanks" dxfId="68" priority="66">
+    <cfRule type="containsBlanks" dxfId="73" priority="71">
       <formula>LEN(TRIM(I194))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I195">
-    <cfRule type="containsBlanks" dxfId="67" priority="65">
+    <cfRule type="containsBlanks" dxfId="72" priority="70">
       <formula>LEN(TRIM(I195))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J195">
-    <cfRule type="containsBlanks" dxfId="66" priority="64">
+    <cfRule type="containsBlanks" dxfId="71" priority="69">
       <formula>LEN(TRIM(J195))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J196">
-    <cfRule type="containsBlanks" dxfId="65" priority="63">
+    <cfRule type="containsBlanks" dxfId="70" priority="68">
       <formula>LEN(TRIM(J196))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I196">
-    <cfRule type="containsBlanks" dxfId="64" priority="62">
+    <cfRule type="containsBlanks" dxfId="69" priority="67">
       <formula>LEN(TRIM(I196))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I197">
-    <cfRule type="containsBlanks" dxfId="63" priority="61">
+    <cfRule type="containsBlanks" dxfId="68" priority="66">
       <formula>LEN(TRIM(I197))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J197">
-    <cfRule type="containsBlanks" dxfId="62" priority="60">
+    <cfRule type="containsBlanks" dxfId="67" priority="65">
       <formula>LEN(TRIM(J197))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C399">
-    <cfRule type="containsBlanks" dxfId="61" priority="59">
+    <cfRule type="containsBlanks" dxfId="66" priority="64">
       <formula>LEN(TRIM(C399))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C400">
-    <cfRule type="containsBlanks" dxfId="60" priority="58">
+    <cfRule type="containsBlanks" dxfId="65" priority="63">
       <formula>LEN(TRIM(C400))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C406">
-    <cfRule type="containsBlanks" dxfId="59" priority="56">
+    <cfRule type="containsBlanks" dxfId="64" priority="61">
       <formula>LEN(TRIM(C406))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D399:D405 D407">
-    <cfRule type="containsBlanks" dxfId="58" priority="55">
+    <cfRule type="containsBlanks" dxfId="63" priority="60">
       <formula>LEN(TRIM(D399))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D406">
-    <cfRule type="containsBlanks" dxfId="57" priority="54">
+    <cfRule type="containsBlanks" dxfId="62" priority="59">
       <formula>LEN(TRIM(D406))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E399:E407">
-    <cfRule type="containsBlanks" dxfId="56" priority="53">
+    <cfRule type="containsBlanks" dxfId="61" priority="58">
       <formula>LEN(TRIM(E399))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F399:F407">
-    <cfRule type="containsBlanks" dxfId="55" priority="52">
+    <cfRule type="containsBlanks" dxfId="60" priority="57">
       <formula>LEN(TRIM(F399))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G401:G407">
-    <cfRule type="containsBlanks" dxfId="54" priority="51">
+    <cfRule type="containsBlanks" dxfId="59" priority="56">
       <formula>LEN(TRIM(G401))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G398">
-    <cfRule type="containsBlanks" dxfId="53" priority="50">
+    <cfRule type="containsBlanks" dxfId="58" priority="55">
       <formula>LEN(TRIM(G398))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H400">
-    <cfRule type="containsBlanks" dxfId="52" priority="49">
+    <cfRule type="containsBlanks" dxfId="57" priority="54">
       <formula>LEN(TRIM(H400))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I398:K407">
-    <cfRule type="containsBlanks" dxfId="51" priority="48">
+    <cfRule type="containsBlanks" dxfId="56" priority="53">
       <formula>LEN(TRIM(I398))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G197">
-    <cfRule type="containsBlanks" dxfId="50" priority="47">
+    <cfRule type="containsBlanks" dxfId="55" priority="52">
       <formula>LEN(TRIM(G197))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C410 C408:G408 K408:K413">
-    <cfRule type="containsBlanks" dxfId="49" priority="46">
+  <conditionalFormatting sqref="C410 C408:G408 K408:K413 K416">
+    <cfRule type="containsBlanks" dxfId="54" priority="51">
       <formula>LEN(TRIM(C408))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E409">
-    <cfRule type="containsBlanks" dxfId="48" priority="45">
+    <cfRule type="containsBlanks" dxfId="53" priority="50">
       <formula>LEN(TRIM(E409))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E410">
-    <cfRule type="containsBlanks" dxfId="47" priority="44">
+    <cfRule type="containsBlanks" dxfId="52" priority="49">
       <formula>LEN(TRIM(E410))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E411">
-    <cfRule type="containsBlanks" dxfId="46" priority="43">
+    <cfRule type="containsBlanks" dxfId="51" priority="48">
       <formula>LEN(TRIM(E411))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E412">
-    <cfRule type="containsBlanks" dxfId="45" priority="42">
+    <cfRule type="containsBlanks" dxfId="50" priority="47">
       <formula>LEN(TRIM(E412))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E413">
-    <cfRule type="containsBlanks" dxfId="44" priority="41">
+    <cfRule type="containsBlanks" dxfId="49" priority="46">
       <formula>LEN(TRIM(E413))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A408:B408">
-    <cfRule type="containsBlanks" dxfId="43" priority="40">
+    <cfRule type="containsBlanks" dxfId="48" priority="45">
       <formula>LEN(TRIM(A408))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A409:B409">
-    <cfRule type="containsBlanks" dxfId="42" priority="39">
+    <cfRule type="containsBlanks" dxfId="47" priority="44">
       <formula>LEN(TRIM(A409))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A410:B410">
-    <cfRule type="containsBlanks" dxfId="41" priority="38">
+    <cfRule type="containsBlanks" dxfId="46" priority="43">
       <formula>LEN(TRIM(A410))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A411:B411">
-    <cfRule type="containsBlanks" dxfId="40" priority="37">
+    <cfRule type="containsBlanks" dxfId="45" priority="42">
       <formula>LEN(TRIM(A411))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A412:B412">
-    <cfRule type="containsBlanks" dxfId="39" priority="36">
+    <cfRule type="containsBlanks" dxfId="44" priority="41">
       <formula>LEN(TRIM(A412))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A413:B413">
-    <cfRule type="containsBlanks" dxfId="38" priority="35">
+    <cfRule type="containsBlanks" dxfId="43" priority="40">
       <formula>LEN(TRIM(A413))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D409">
-    <cfRule type="containsBlanks" dxfId="37" priority="34">
+    <cfRule type="containsBlanks" dxfId="42" priority="39">
       <formula>LEN(TRIM(D409))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D411">
-    <cfRule type="containsBlanks" dxfId="36" priority="33">
+    <cfRule type="containsBlanks" dxfId="41" priority="38">
       <formula>LEN(TRIM(D411))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D412">
-    <cfRule type="containsBlanks" dxfId="35" priority="32">
+    <cfRule type="containsBlanks" dxfId="40" priority="37">
       <formula>LEN(TRIM(D412))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C409">
-    <cfRule type="containsBlanks" dxfId="34" priority="31">
+    <cfRule type="containsBlanks" dxfId="39" priority="36">
       <formula>LEN(TRIM(C409))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C411">
-    <cfRule type="containsBlanks" dxfId="33" priority="30">
+    <cfRule type="containsBlanks" dxfId="38" priority="35">
       <formula>LEN(TRIM(C411))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C412">
-    <cfRule type="containsBlanks" dxfId="32" priority="29">
+    <cfRule type="containsBlanks" dxfId="37" priority="34">
       <formula>LEN(TRIM(C412))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C413">
-    <cfRule type="containsBlanks" dxfId="31" priority="28">
+    <cfRule type="containsBlanks" dxfId="36" priority="33">
       <formula>LEN(TRIM(C413))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F409">
-    <cfRule type="containsBlanks" dxfId="30" priority="27">
+    <cfRule type="containsBlanks" dxfId="35" priority="32">
       <formula>LEN(TRIM(F409))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F410">
-    <cfRule type="containsBlanks" dxfId="29" priority="26">
+    <cfRule type="containsBlanks" dxfId="34" priority="31">
       <formula>LEN(TRIM(F410))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F411">
-    <cfRule type="containsBlanks" dxfId="28" priority="25">
+    <cfRule type="containsBlanks" dxfId="33" priority="30">
       <formula>LEN(TRIM(F411))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F412">
-    <cfRule type="containsBlanks" dxfId="27" priority="24">
+    <cfRule type="containsBlanks" dxfId="32" priority="29">
       <formula>LEN(TRIM(F412))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F413">
-    <cfRule type="containsBlanks" dxfId="26" priority="23">
+    <cfRule type="containsBlanks" dxfId="31" priority="28">
       <formula>LEN(TRIM(F413))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H408">
-    <cfRule type="containsBlanks" dxfId="25" priority="22">
+    <cfRule type="containsBlanks" dxfId="30" priority="27">
       <formula>LEN(TRIM(H408))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H409">
-    <cfRule type="containsBlanks" dxfId="24" priority="21">
+    <cfRule type="containsBlanks" dxfId="29" priority="26">
       <formula>LEN(TRIM(H409))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H410">
-    <cfRule type="containsBlanks" dxfId="23" priority="20">
+    <cfRule type="containsBlanks" dxfId="28" priority="25">
       <formula>LEN(TRIM(H410))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H411">
-    <cfRule type="containsBlanks" dxfId="22" priority="19">
+    <cfRule type="containsBlanks" dxfId="27" priority="24">
       <formula>LEN(TRIM(H411))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H412">
-    <cfRule type="containsBlanks" dxfId="21" priority="18">
+    <cfRule type="containsBlanks" dxfId="26" priority="23">
       <formula>LEN(TRIM(H412))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H413">
-    <cfRule type="containsBlanks" dxfId="20" priority="17">
+    <cfRule type="containsBlanks" dxfId="25" priority="22">
       <formula>LEN(TRIM(H413))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G409">
-    <cfRule type="containsBlanks" dxfId="19" priority="16">
+    <cfRule type="containsBlanks" dxfId="24" priority="21">
       <formula>LEN(TRIM(G409))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G410">
-    <cfRule type="containsBlanks" dxfId="18" priority="15">
+    <cfRule type="containsBlanks" dxfId="23" priority="20">
       <formula>LEN(TRIM(G410))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G411">
-    <cfRule type="containsBlanks" dxfId="17" priority="14">
+    <cfRule type="containsBlanks" dxfId="22" priority="19">
       <formula>LEN(TRIM(G411))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G412">
-    <cfRule type="containsBlanks" dxfId="16" priority="13">
+    <cfRule type="containsBlanks" dxfId="21" priority="18">
       <formula>LEN(TRIM(G412))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G413">
-    <cfRule type="containsBlanks" dxfId="15" priority="12">
+    <cfRule type="containsBlanks" dxfId="20" priority="17">
       <formula>LEN(TRIM(G413))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K414:K415">
-    <cfRule type="containsBlanks" dxfId="14" priority="11">
+    <cfRule type="containsBlanks" dxfId="19" priority="16">
       <formula>LEN(TRIM(K414))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A414:B414">
-    <cfRule type="containsBlanks" dxfId="13" priority="10">
+    <cfRule type="containsBlanks" dxfId="18" priority="15">
       <formula>LEN(TRIM(A414))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A415:B415">
-    <cfRule type="containsBlanks" dxfId="12" priority="9">
+  <conditionalFormatting sqref="A415:B415 A416:A429">
+    <cfRule type="containsBlanks" dxfId="17" priority="14">
       <formula>LEN(TRIM(A415))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C414">
-    <cfRule type="containsBlanks" dxfId="11" priority="8">
+    <cfRule type="containsBlanks" dxfId="16" priority="13">
       <formula>LEN(TRIM(C414))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C415">
-    <cfRule type="containsBlanks" dxfId="10" priority="7">
+    <cfRule type="containsBlanks" dxfId="15" priority="12">
       <formula>LEN(TRIM(C415))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:K8">
-    <cfRule type="containsBlanks" dxfId="9" priority="6">
+    <cfRule type="containsBlanks" dxfId="14" priority="11">
       <formula>LEN(TRIM(A8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:K7">
-    <cfRule type="containsBlanks" dxfId="7" priority="5">
+    <cfRule type="containsBlanks" dxfId="12" priority="10">
       <formula>LEN(TRIM(F7))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:K6">
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
+  <conditionalFormatting sqref="A6:F6 I6:K6">
+    <cfRule type="containsBlanks" dxfId="11" priority="9">
       <formula>LEN(TRIM(A6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:K5">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
+    <cfRule type="containsBlanks" dxfId="8" priority="8">
       <formula>LEN(TRIM(A5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:K4">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
+    <cfRule type="containsBlanks" dxfId="7" priority="7">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:K3">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B416:B429">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(B416))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K417:K429">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(K417))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(H6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A3))=0</formula>
+      <formula>LEN(TRIM(G6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17616,7 +18242,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I17">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="6" priority="1">
       <formula>LEN(TRIM(I17))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
92%! :)))) Let's pick this back up tomorrow
</commit_message>
<xml_diff>
--- a/test_constraints.xlsx
+++ b/test_constraints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HumeD\PycharmProjects\Data_Profile_Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D15C220-2A0C-42EA-BB0D-2F97B929D50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECD99EA-8AE0-4CA7-A52D-935F0A5100BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{D2E9D144-5D6F-4AC1-9DA3-D4FF634D9598}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Data Set Definitions" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Constraint Definitions'!$D$1:$D$407</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Constraint Definitions'!$D$1:$D$405</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3048" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3059" uniqueCount="532">
   <si>
     <t>Constraint_Set_Name</t>
   </si>
@@ -1378,9 +1378,6 @@
     <t>C364Known Errors: D_I_L defined when it shouldn’t be</t>
   </si>
   <si>
-    <t>C365Known Errors: Element not defined when it should be</t>
-  </si>
-  <si>
     <t>C366Known Errors: Measure_Index defined when it shouldn’t be</t>
   </si>
   <si>
@@ -1429,9 +1426,6 @@
     <t>C381Known Errors: D_I_L defined when it shouldn’t be</t>
   </si>
   <si>
-    <t>C382Known Errors: Element not defined when it should be</t>
-  </si>
-  <si>
     <t>C383Known Errors: Measure_Index defined when it shouldn’t be</t>
   </si>
   <si>
@@ -1613,6 +1607,36 @@
   </si>
   <si>
     <t>inf</t>
+  </si>
+  <si>
+    <t>STS0</t>
+  </si>
+  <si>
+    <t>Empty Relative Data Set</t>
+  </si>
+  <si>
+    <t>C422PASS: Absolute Column Name</t>
+  </si>
+  <si>
+    <t>Empty Primary Data Set</t>
+  </si>
+  <si>
+    <t>PTS0</t>
+  </si>
+  <si>
+    <t>C423PASS: Absolute Header</t>
+  </si>
+  <si>
+    <t>C:/sandbox/data/raw/Data_Profile_Tester/sts0.dat</t>
+  </si>
+  <si>
+    <t>C:/sandbox/data/raw/Data_Profile_Tester/pts0.dat</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>X,X</t>
   </si>
 </sst>
 </file>
@@ -1676,21 +1700,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="85">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="83">
     <dxf>
       <fill>
         <patternFill>
@@ -2590,7 +2600,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2634,17 +2644,33 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>530</v>
+      </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>530</v>
+      </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2820,8 +2846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E86614-3B97-43D1-B6C4-36CEB2305CDA}">
   <dimension ref="A1:K429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
+      <selection activeCell="A389" sqref="A389:XFD389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2884,13 +2910,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F3" t="s">
         <v>49</v>
@@ -2919,13 +2945,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F4" t="s">
         <v>49</v>
@@ -2954,10 +2980,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>68</v>
@@ -2966,7 +2992,7 @@
         <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
@@ -2989,7 +3015,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>45</v>
@@ -3021,7 +3047,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D7" t="s">
         <v>45</v>
@@ -3056,7 +3082,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>43</v>
@@ -3074,10 +3100,10 @@
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="J8" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -4713,13 +4739,13 @@
         <v>49</v>
       </c>
       <c r="G55" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="H55" t="s">
         <v>21</v>
       </c>
-      <c r="I55">
-        <v>0</v>
+      <c r="I55" t="s">
+        <v>21</v>
       </c>
       <c r="J55">
         <v>100</v>
@@ -5168,7 +5194,7 @@
         <v>49</v>
       </c>
       <c r="G68" t="s">
-        <v>72</v>
+        <v>531</v>
       </c>
       <c r="H68">
         <v>3</v>
@@ -5413,10 +5439,10 @@
         <v>49</v>
       </c>
       <c r="G75" t="s">
-        <v>72</v>
-      </c>
-      <c r="H75">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="H75" t="s">
+        <v>21</v>
       </c>
       <c r="I75" t="s">
         <v>21</v>
@@ -6381,7 +6407,7 @@
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>44</v>
@@ -9018,7 +9044,7 @@
         <v>21</v>
       </c>
       <c r="G178" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="H178" t="s">
         <v>21</v>
@@ -9298,7 +9324,7 @@
         <v>21</v>
       </c>
       <c r="G186" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="H186" t="s">
         <v>21</v>
@@ -9753,7 +9779,7 @@
         <v>21</v>
       </c>
       <c r="G199" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="H199" t="s">
         <v>21</v>
@@ -12346,7 +12372,7 @@
         <v>72</v>
       </c>
       <c r="H273">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I273">
         <v>1</v>
@@ -15729,7 +15755,7 @@
         <v>442</v>
       </c>
       <c r="D370" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E370" s="2" t="s">
         <v>65</v>
@@ -15764,7 +15790,7 @@
         <v>443</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E371" s="2" t="s">
         <v>65</v>
@@ -15845,8 +15871,8 @@
       <c r="G373" t="s">
         <v>21</v>
       </c>
-      <c r="H373" t="s">
-        <v>21</v>
+      <c r="H373">
+        <v>3</v>
       </c>
       <c r="I373" t="s">
         <v>21</v>
@@ -15880,11 +15906,11 @@
       <c r="G374" t="s">
         <v>21</v>
       </c>
-      <c r="H374">
-        <v>3</v>
-      </c>
-      <c r="I374" t="s">
-        <v>21</v>
+      <c r="H374" t="s">
+        <v>21</v>
+      </c>
+      <c r="I374">
+        <v>1</v>
       </c>
       <c r="J374" t="s">
         <v>21</v>
@@ -15918,11 +15944,11 @@
       <c r="H375" t="s">
         <v>21</v>
       </c>
-      <c r="I375">
-        <v>1</v>
-      </c>
-      <c r="J375" t="s">
-        <v>21</v>
+      <c r="I375" t="s">
+        <v>21</v>
+      </c>
+      <c r="J375">
+        <v>1</v>
       </c>
       <c r="K375">
         <v>1</v>
@@ -15956,11 +15982,11 @@
       <c r="I376" t="s">
         <v>21</v>
       </c>
-      <c r="J376">
-        <v>1</v>
-      </c>
-      <c r="K376">
-        <v>1</v>
+      <c r="J376" t="s">
+        <v>21</v>
+      </c>
+      <c r="K376" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="377" spans="1:11" x14ac:dyDescent="0.25">
@@ -15974,7 +16000,7 @@
         <v>449</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E377" s="2" t="s">
         <v>66</v>
@@ -15994,8 +16020,8 @@
       <c r="J377" t="s">
         <v>21</v>
       </c>
-      <c r="K377" t="s">
-        <v>21</v>
+      <c r="K377">
+        <v>1</v>
       </c>
     </row>
     <row r="378" spans="1:11" x14ac:dyDescent="0.25">
@@ -16044,7 +16070,7 @@
         <v>451</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E379" s="2" t="s">
         <v>66</v>
@@ -16079,19 +16105,19 @@
         <v>452</v>
       </c>
       <c r="D380" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E380" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F380" t="s">
-        <v>21</v>
-      </c>
-      <c r="G380" t="s">
-        <v>21</v>
-      </c>
-      <c r="H380" t="s">
-        <v>21</v>
+        <v>67</v>
+      </c>
+      <c r="F380" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G380" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H380">
+        <v>3</v>
       </c>
       <c r="I380" t="s">
         <v>21</v>
@@ -16120,10 +16146,10 @@
         <v>67</v>
       </c>
       <c r="F381" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G381" s="2" t="s">
-        <v>21</v>
+        <v>21</v>
+      </c>
+      <c r="G381" t="s">
+        <v>41</v>
       </c>
       <c r="H381">
         <v>3</v>
@@ -16157,11 +16183,11 @@
       <c r="F382" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G382" t="s">
-        <v>41</v>
-      </c>
-      <c r="H382">
-        <v>3</v>
+      <c r="G382" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H382" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="I382" t="s">
         <v>21</v>
@@ -16195,11 +16221,11 @@
       <c r="G383" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H383" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I383" t="s">
-        <v>21</v>
+      <c r="H383">
+        <v>3</v>
+      </c>
+      <c r="I383">
+        <v>1</v>
       </c>
       <c r="J383" t="s">
         <v>21</v>
@@ -16233,11 +16259,11 @@
       <c r="H384">
         <v>3</v>
       </c>
-      <c r="I384">
-        <v>1</v>
-      </c>
-      <c r="J384" t="s">
-        <v>21</v>
+      <c r="I384" t="s">
+        <v>21</v>
+      </c>
+      <c r="J384">
+        <v>1</v>
       </c>
       <c r="K384">
         <v>1</v>
@@ -16271,11 +16297,11 @@
       <c r="I385" t="s">
         <v>21</v>
       </c>
-      <c r="J385">
-        <v>1</v>
-      </c>
-      <c r="K385">
-        <v>1</v>
+      <c r="J385" t="s">
+        <v>21</v>
+      </c>
+      <c r="K385" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="386" spans="1:11" x14ac:dyDescent="0.25">
@@ -16289,7 +16315,7 @@
         <v>458</v>
       </c>
       <c r="D386" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E386" s="2" t="s">
         <v>67</v>
@@ -16309,8 +16335,8 @@
       <c r="J386" t="s">
         <v>21</v>
       </c>
-      <c r="K386" t="s">
-        <v>21</v>
+      <c r="K386">
+        <v>1</v>
       </c>
     </row>
     <row r="387" spans="1:11" x14ac:dyDescent="0.25">
@@ -16324,7 +16350,7 @@
         <v>459</v>
       </c>
       <c r="D387" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E387" s="2" t="s">
         <v>67</v>
@@ -16362,16 +16388,16 @@
         <v>45</v>
       </c>
       <c r="E388" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F388" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G388" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H388">
-        <v>3</v>
+        <v>68</v>
+      </c>
+      <c r="F388" t="s">
+        <v>49</v>
+      </c>
+      <c r="G388" t="s">
+        <v>21</v>
+      </c>
+      <c r="H388" t="s">
+        <v>21</v>
       </c>
       <c r="I388" t="s">
         <v>21</v>
@@ -16400,13 +16426,13 @@
         <v>68</v>
       </c>
       <c r="F389" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="G389" t="s">
         <v>21</v>
       </c>
-      <c r="H389" t="s">
-        <v>21</v>
+      <c r="H389">
+        <v>3</v>
       </c>
       <c r="I389" t="s">
         <v>21</v>
@@ -16443,8 +16469,8 @@
       <c r="H390" t="s">
         <v>21</v>
       </c>
-      <c r="I390" t="s">
-        <v>21</v>
+      <c r="I390">
+        <v>1</v>
       </c>
       <c r="J390" t="s">
         <v>21</v>
@@ -16475,14 +16501,14 @@
       <c r="G391" t="s">
         <v>21</v>
       </c>
-      <c r="H391">
-        <v>3</v>
+      <c r="H391" t="s">
+        <v>21</v>
       </c>
       <c r="I391" t="s">
         <v>21</v>
       </c>
-      <c r="J391" t="s">
-        <v>21</v>
+      <c r="J391">
+        <v>1</v>
       </c>
       <c r="K391">
         <v>1</v>
@@ -16513,14 +16539,14 @@
       <c r="H392" t="s">
         <v>21</v>
       </c>
-      <c r="I392">
-        <v>1</v>
+      <c r="I392" t="s">
+        <v>21</v>
       </c>
       <c r="J392" t="s">
         <v>21</v>
       </c>
-      <c r="K392">
-        <v>1</v>
+      <c r="K392" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="393" spans="1:11" x14ac:dyDescent="0.25">
@@ -16534,7 +16560,7 @@
         <v>465</v>
       </c>
       <c r="D393" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E393" s="2" t="s">
         <v>68</v>
@@ -16551,8 +16577,8 @@
       <c r="I393" t="s">
         <v>21</v>
       </c>
-      <c r="J393">
-        <v>1</v>
+      <c r="J393" t="s">
+        <v>21</v>
       </c>
       <c r="K393">
         <v>1</v>
@@ -16569,7 +16595,7 @@
         <v>466</v>
       </c>
       <c r="D394" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E394" s="2" t="s">
         <v>68</v>
@@ -16589,8 +16615,8 @@
       <c r="J394" t="s">
         <v>21</v>
       </c>
-      <c r="K394" t="s">
-        <v>21</v>
+      <c r="K394">
+        <v>1</v>
       </c>
     </row>
     <row r="395" spans="1:11" x14ac:dyDescent="0.25">
@@ -16604,7 +16630,7 @@
         <v>467</v>
       </c>
       <c r="D395" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E395" s="2" t="s">
         <v>68</v>
@@ -16639,19 +16665,19 @@
         <v>468</v>
       </c>
       <c r="D396" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E396" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F396" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F396" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="G396" t="s">
         <v>21</v>
       </c>
-      <c r="H396" t="s">
-        <v>21</v>
+      <c r="H396">
+        <v>3</v>
       </c>
       <c r="I396" t="s">
         <v>21</v>
@@ -16674,19 +16700,19 @@
         <v>469</v>
       </c>
       <c r="D397" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E397" s="2" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="F397" t="s">
         <v>21</v>
       </c>
       <c r="G397" t="s">
-        <v>21</v>
-      </c>
-      <c r="H397" t="s">
-        <v>21</v>
+        <v>48</v>
+      </c>
+      <c r="H397">
+        <v>3</v>
       </c>
       <c r="I397" t="s">
         <v>21</v>
@@ -16714,14 +16740,14 @@
       <c r="E398" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F398" s="2" t="s">
-        <v>49</v>
+      <c r="F398" t="s">
+        <v>21</v>
       </c>
       <c r="G398" t="s">
         <v>21</v>
       </c>
-      <c r="H398">
-        <v>3</v>
+      <c r="H398" t="s">
+        <v>21</v>
       </c>
       <c r="I398" t="s">
         <v>21</v>
@@ -16753,7 +16779,7 @@
         <v>21</v>
       </c>
       <c r="G399" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="H399">
         <v>3</v>
@@ -16790,8 +16816,8 @@
       <c r="G400" t="s">
         <v>21</v>
       </c>
-      <c r="H400" t="s">
-        <v>21</v>
+      <c r="H400">
+        <v>3</v>
       </c>
       <c r="I400" t="s">
         <v>21</v>
@@ -16834,8 +16860,8 @@
       <c r="J401" t="s">
         <v>21</v>
       </c>
-      <c r="K401">
-        <v>1</v>
+      <c r="K401" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="402" spans="1:11" x14ac:dyDescent="0.25">
@@ -16884,7 +16910,7 @@
         <v>475</v>
       </c>
       <c r="D403" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E403" s="2" t="s">
         <v>19</v>
@@ -16898,14 +16924,14 @@
       <c r="H403">
         <v>3</v>
       </c>
-      <c r="I403" t="s">
-        <v>21</v>
-      </c>
-      <c r="J403" t="s">
-        <v>21</v>
-      </c>
-      <c r="K403" t="s">
-        <v>21</v>
+      <c r="I403">
+        <v>0.25</v>
+      </c>
+      <c r="J403">
+        <v>0.75</v>
+      </c>
+      <c r="K403">
+        <v>1</v>
       </c>
     </row>
     <row r="404" spans="1:11" x14ac:dyDescent="0.25">
@@ -16919,7 +16945,7 @@
         <v>476</v>
       </c>
       <c r="D404" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E404" s="2" t="s">
         <v>19</v>
@@ -16933,11 +16959,11 @@
       <c r="H404">
         <v>3</v>
       </c>
-      <c r="I404" t="s">
-        <v>21</v>
-      </c>
-      <c r="J404" t="s">
-        <v>21</v>
+      <c r="I404">
+        <v>0.25</v>
+      </c>
+      <c r="J404">
+        <v>0.75</v>
       </c>
       <c r="K404">
         <v>1</v>
@@ -16950,11 +16976,11 @@
       <c r="B405">
         <v>1</v>
       </c>
-      <c r="C405" t="s">
+      <c r="C405" s="3" t="s">
         <v>477</v>
       </c>
       <c r="D405" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E405" s="2" t="s">
         <v>19</v>
@@ -16972,7 +16998,7 @@
         <v>0.25</v>
       </c>
       <c r="J405">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="K405">
         <v>1</v>
@@ -16988,26 +17014,26 @@
       <c r="C406" t="s">
         <v>478</v>
       </c>
-      <c r="D406" s="2" t="s">
+      <c r="D406" t="s">
         <v>44</v>
       </c>
-      <c r="E406" s="2" t="s">
-        <v>19</v>
+      <c r="E406" t="s">
+        <v>79</v>
       </c>
       <c r="F406" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="G406" t="s">
-        <v>21</v>
-      </c>
-      <c r="H406">
-        <v>3</v>
+        <v>72</v>
+      </c>
+      <c r="H406" t="s">
+        <v>21</v>
       </c>
       <c r="I406">
-        <v>0.25</v>
+        <v>11</v>
       </c>
       <c r="J406">
-        <v>0.75</v>
+        <v>20</v>
       </c>
       <c r="K406">
         <v>1</v>
@@ -17020,29 +17046,29 @@
       <c r="B407">
         <v>1</v>
       </c>
-      <c r="C407" s="3" t="s">
+      <c r="C407" t="s">
         <v>479</v>
       </c>
-      <c r="D407" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E407" s="2" t="s">
-        <v>19</v>
+      <c r="D407" t="s">
+        <v>44</v>
+      </c>
+      <c r="E407" t="s">
+        <v>79</v>
       </c>
       <c r="F407" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="G407" t="s">
-        <v>21</v>
-      </c>
-      <c r="H407">
-        <v>3</v>
+        <v>72</v>
+      </c>
+      <c r="H407" t="s">
+        <v>21</v>
       </c>
       <c r="I407">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="J407">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K407">
         <v>1</v>
@@ -17059,7 +17085,7 @@
         <v>480</v>
       </c>
       <c r="D408" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E408" t="s">
         <v>79</v>
@@ -17074,10 +17100,10 @@
         <v>21</v>
       </c>
       <c r="I408">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J408">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K408">
         <v>1</v>
@@ -17097,7 +17123,7 @@
         <v>44</v>
       </c>
       <c r="E409" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F409" t="s">
         <v>71</v>
@@ -17109,10 +17135,10 @@
         <v>21</v>
       </c>
       <c r="I409">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J409">
-        <v>9</v>
+        <v>0.5</v>
       </c>
       <c r="K409">
         <v>1</v>
@@ -17129,10 +17155,10 @@
         <v>482</v>
       </c>
       <c r="D410" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E410" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F410" t="s">
         <v>71</v>
@@ -17144,10 +17170,10 @@
         <v>21</v>
       </c>
       <c r="I410">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="J410">
-        <v>10</v>
+        <v>0.8</v>
       </c>
       <c r="K410">
         <v>1</v>
@@ -17164,7 +17190,7 @@
         <v>483</v>
       </c>
       <c r="D411" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E411" t="s">
         <v>80</v>
@@ -17179,10 +17205,10 @@
         <v>21</v>
       </c>
       <c r="I411">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J411">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K411">
         <v>1</v>
@@ -17202,22 +17228,22 @@
         <v>44</v>
       </c>
       <c r="E412" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="F412" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="G412" t="s">
-        <v>72</v>
-      </c>
-      <c r="H412" t="s">
-        <v>21</v>
-      </c>
-      <c r="I412">
-        <v>0.5</v>
-      </c>
-      <c r="J412">
-        <v>0.8</v>
+        <v>21</v>
+      </c>
+      <c r="H412">
+        <v>0</v>
+      </c>
+      <c r="I412" t="s">
+        <v>21</v>
+      </c>
+      <c r="J412" t="s">
+        <v>21</v>
       </c>
       <c r="K412">
         <v>1</v>
@@ -17237,22 +17263,22 @@
         <v>43</v>
       </c>
       <c r="E413" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="F413" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="G413" t="s">
-        <v>72</v>
-      </c>
-      <c r="H413" t="s">
-        <v>21</v>
-      </c>
-      <c r="I413">
-        <v>1</v>
-      </c>
-      <c r="J413">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="H413">
+        <v>0</v>
+      </c>
+      <c r="I413" t="s">
+        <v>21</v>
+      </c>
+      <c r="J413" t="s">
+        <v>21</v>
       </c>
       <c r="K413">
         <v>1</v>
@@ -17266,13 +17292,13 @@
         <v>1</v>
       </c>
       <c r="C414" t="s">
-        <v>486</v>
+        <v>507</v>
       </c>
       <c r="D414" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E414" t="s">
-        <v>67</v>
+        <v>497</v>
       </c>
       <c r="F414" t="s">
         <v>21</v>
@@ -17283,11 +17309,11 @@
       <c r="H414">
         <v>0</v>
       </c>
-      <c r="I414" t="s">
-        <v>21</v>
-      </c>
-      <c r="J414" t="s">
-        <v>21</v>
+      <c r="I414">
+        <v>1</v>
+      </c>
+      <c r="J414">
+        <v>1</v>
       </c>
       <c r="K414">
         <v>1</v>
@@ -17301,13 +17327,13 @@
         <v>1</v>
       </c>
       <c r="C415" t="s">
-        <v>487</v>
+        <v>516</v>
       </c>
       <c r="D415" t="s">
         <v>43</v>
       </c>
       <c r="E415" t="s">
-        <v>67</v>
+        <v>498</v>
       </c>
       <c r="F415" t="s">
         <v>21</v>
@@ -17318,11 +17344,11 @@
       <c r="H415">
         <v>0</v>
       </c>
-      <c r="I415" t="s">
-        <v>21</v>
-      </c>
-      <c r="J415" t="s">
-        <v>21</v>
+      <c r="I415">
+        <v>1</v>
+      </c>
+      <c r="J415">
+        <v>1</v>
       </c>
       <c r="K415">
         <v>1</v>
@@ -17336,7 +17362,7 @@
         <v>1</v>
       </c>
       <c r="C416" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D416" t="s">
         <v>43</v>
@@ -17351,13 +17377,13 @@
         <v>21</v>
       </c>
       <c r="H416">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I416">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J416">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K416">
         <v>1</v>
@@ -17371,7 +17397,7 @@
         <v>1</v>
       </c>
       <c r="C417" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D417" t="s">
         <v>43</v>
@@ -17386,7 +17412,7 @@
         <v>21</v>
       </c>
       <c r="H417">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I417">
         <v>1</v>
@@ -17406,7 +17432,7 @@
         <v>1</v>
       </c>
       <c r="C418" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D418" t="s">
         <v>43</v>
@@ -17441,7 +17467,7 @@
         <v>1</v>
       </c>
       <c r="C419" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D419" t="s">
         <v>43</v>
@@ -17476,7 +17502,7 @@
         <v>1</v>
       </c>
       <c r="C420" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D420" t="s">
         <v>43</v>
@@ -17491,13 +17517,13 @@
         <v>21</v>
       </c>
       <c r="H420">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I420">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J420">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K420">
         <v>1</v>
@@ -17511,7 +17537,7 @@
         <v>1</v>
       </c>
       <c r="C421" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D421" t="s">
         <v>43</v>
@@ -17526,7 +17552,7 @@
         <v>21</v>
       </c>
       <c r="H421">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I421">
         <v>1</v>
@@ -17546,7 +17572,7 @@
         <v>1</v>
       </c>
       <c r="C422" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D422" t="s">
         <v>43</v>
@@ -17581,7 +17607,7 @@
         <v>1</v>
       </c>
       <c r="C423" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D423" t="s">
         <v>43</v>
@@ -17616,28 +17642,28 @@
         <v>1</v>
       </c>
       <c r="C424" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="D424" t="s">
         <v>43</v>
       </c>
       <c r="E424" t="s">
-        <v>507</v>
+        <v>59</v>
       </c>
       <c r="F424" t="s">
         <v>21</v>
       </c>
       <c r="G424" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="H424">
-        <v>6</v>
-      </c>
-      <c r="I424">
-        <v>10</v>
-      </c>
-      <c r="J424">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="I424" t="s">
+        <v>21</v>
+      </c>
+      <c r="J424" t="s">
+        <v>21</v>
       </c>
       <c r="K424">
         <v>1</v>
@@ -17651,13 +17677,13 @@
         <v>1</v>
       </c>
       <c r="C425" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="D425" t="s">
         <v>43</v>
       </c>
       <c r="E425" t="s">
-        <v>508</v>
+        <v>65</v>
       </c>
       <c r="F425" t="s">
         <v>21</v>
@@ -17666,13 +17692,13 @@
         <v>21</v>
       </c>
       <c r="H425">
-        <v>6</v>
-      </c>
-      <c r="I425">
-        <v>1</v>
-      </c>
-      <c r="J425">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I425" t="s">
+        <v>21</v>
+      </c>
+      <c r="J425" t="s">
+        <v>21</v>
       </c>
       <c r="K425">
         <v>1</v>
@@ -17692,13 +17718,13 @@
         <v>43</v>
       </c>
       <c r="E426" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F426" t="s">
         <v>21</v>
       </c>
       <c r="G426" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H426">
         <v>0</v>
@@ -17727,7 +17753,7 @@
         <v>43</v>
       </c>
       <c r="E427" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F427" t="s">
         <v>21</v>
@@ -17749,14 +17775,14 @@
       </c>
     </row>
     <row r="428" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A428" s="1" t="s">
-        <v>78</v>
+      <c r="A428" s="4" t="s">
+        <v>523</v>
       </c>
       <c r="B428">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C428" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="D428" t="s">
         <v>43</v>
@@ -17784,29 +17810,29 @@
       </c>
     </row>
     <row r="429" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A429" s="1" t="s">
-        <v>78</v>
+      <c r="A429" t="s">
+        <v>525</v>
       </c>
       <c r="B429">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C429" t="s">
-        <v>522</v>
-      </c>
-      <c r="D429" t="s">
+        <v>527</v>
+      </c>
+      <c r="D429" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E429" t="s">
-        <v>67</v>
+      <c r="E429" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="F429" t="s">
         <v>21</v>
       </c>
       <c r="G429" t="s">
-        <v>21</v>
-      </c>
-      <c r="H429">
-        <v>0</v>
+        <v>77</v>
+      </c>
+      <c r="H429" t="s">
+        <v>21</v>
       </c>
       <c r="I429" t="s">
         <v>21</v>
@@ -17820,404 +17846,414 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="C193:K193 J194:K194 K195:K197 C401:C405 C407 C398:F398 G399:G400 C194:H195 C197:F197 C196:G196 H196:H197 C9:K189 A9:B407 C198:K397 A1:K2 A7:E7">
-    <cfRule type="containsBlanks" dxfId="84" priority="82">
+  <conditionalFormatting sqref="C193:K193 J194:K194 K195:K197 C399:C403 C405 C396:F396 G397:G398 C194:H195 C197:F197 C196:G196 H196:H197 A1:K2 A7:E7 C9:K189 A9:B405 C198:K395">
+    <cfRule type="containsBlanks" dxfId="82" priority="84">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C190:C192">
-    <cfRule type="containsBlanks" dxfId="83" priority="81">
+    <cfRule type="containsBlanks" dxfId="81" priority="83">
       <formula>LEN(TRIM(C190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D190">
-    <cfRule type="containsBlanks" dxfId="82" priority="80">
+    <cfRule type="containsBlanks" dxfId="80" priority="82">
       <formula>LEN(TRIM(D190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="containsBlanks" dxfId="81" priority="79">
+    <cfRule type="containsBlanks" dxfId="79" priority="81">
       <formula>LEN(TRIM(D191))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D192">
-    <cfRule type="containsBlanks" dxfId="80" priority="78">
+    <cfRule type="containsBlanks" dxfId="78" priority="80">
       <formula>LEN(TRIM(D192))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E190">
-    <cfRule type="containsBlanks" dxfId="79" priority="77">
+    <cfRule type="containsBlanks" dxfId="77" priority="79">
       <formula>LEN(TRIM(E190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E191">
-    <cfRule type="containsBlanks" dxfId="78" priority="76">
+    <cfRule type="containsBlanks" dxfId="76" priority="78">
       <formula>LEN(TRIM(E191))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E192">
-    <cfRule type="containsBlanks" dxfId="77" priority="75">
+    <cfRule type="containsBlanks" dxfId="75" priority="77">
       <formula>LEN(TRIM(E192))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F190:K190">
-    <cfRule type="containsBlanks" dxfId="76" priority="74">
+    <cfRule type="containsBlanks" dxfId="74" priority="76">
       <formula>LEN(TRIM(F190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F191:K191">
-    <cfRule type="containsBlanks" dxfId="75" priority="73">
+    <cfRule type="containsBlanks" dxfId="73" priority="75">
       <formula>LEN(TRIM(F191))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F192:K192">
-    <cfRule type="containsBlanks" dxfId="74" priority="72">
+    <cfRule type="containsBlanks" dxfId="72" priority="74">
       <formula>LEN(TRIM(F192))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I194">
-    <cfRule type="containsBlanks" dxfId="73" priority="71">
+    <cfRule type="containsBlanks" dxfId="71" priority="73">
       <formula>LEN(TRIM(I194))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I195">
-    <cfRule type="containsBlanks" dxfId="72" priority="70">
+    <cfRule type="containsBlanks" dxfId="70" priority="72">
       <formula>LEN(TRIM(I195))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J195">
-    <cfRule type="containsBlanks" dxfId="71" priority="69">
+    <cfRule type="containsBlanks" dxfId="69" priority="71">
       <formula>LEN(TRIM(J195))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J196">
-    <cfRule type="containsBlanks" dxfId="70" priority="68">
+    <cfRule type="containsBlanks" dxfId="68" priority="70">
       <formula>LEN(TRIM(J196))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I196">
-    <cfRule type="containsBlanks" dxfId="69" priority="67">
+    <cfRule type="containsBlanks" dxfId="67" priority="69">
       <formula>LEN(TRIM(I196))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I197">
-    <cfRule type="containsBlanks" dxfId="68" priority="66">
+    <cfRule type="containsBlanks" dxfId="66" priority="68">
       <formula>LEN(TRIM(I197))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J197">
-    <cfRule type="containsBlanks" dxfId="67" priority="65">
+    <cfRule type="containsBlanks" dxfId="65" priority="67">
       <formula>LEN(TRIM(J197))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C399">
-    <cfRule type="containsBlanks" dxfId="66" priority="64">
-      <formula>LEN(TRIM(C399))=0</formula>
+  <conditionalFormatting sqref="C397">
+    <cfRule type="containsBlanks" dxfId="64" priority="66">
+      <formula>LEN(TRIM(C397))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C400">
-    <cfRule type="containsBlanks" dxfId="65" priority="63">
-      <formula>LEN(TRIM(C400))=0</formula>
+  <conditionalFormatting sqref="C398">
+    <cfRule type="containsBlanks" dxfId="63" priority="65">
+      <formula>LEN(TRIM(C398))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C406">
-    <cfRule type="containsBlanks" dxfId="64" priority="61">
+  <conditionalFormatting sqref="C404">
+    <cfRule type="containsBlanks" dxfId="62" priority="63">
+      <formula>LEN(TRIM(C404))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D397:D403 D405">
+    <cfRule type="containsBlanks" dxfId="61" priority="62">
+      <formula>LEN(TRIM(D397))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D404">
+    <cfRule type="containsBlanks" dxfId="60" priority="61">
+      <formula>LEN(TRIM(D404))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E397:E405">
+    <cfRule type="containsBlanks" dxfId="59" priority="60">
+      <formula>LEN(TRIM(E397))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F397:F405">
+    <cfRule type="containsBlanks" dxfId="58" priority="59">
+      <formula>LEN(TRIM(F397))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G399:G405">
+    <cfRule type="containsBlanks" dxfId="57" priority="58">
+      <formula>LEN(TRIM(G399))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G396">
+    <cfRule type="containsBlanks" dxfId="56" priority="57">
+      <formula>LEN(TRIM(G396))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H398">
+    <cfRule type="containsBlanks" dxfId="55" priority="56">
+      <formula>LEN(TRIM(H398))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I396:K405">
+    <cfRule type="containsBlanks" dxfId="54" priority="55">
+      <formula>LEN(TRIM(I396))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G197">
+    <cfRule type="containsBlanks" dxfId="53" priority="54">
+      <formula>LEN(TRIM(G197))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C408 C406:G406 K406:K411 K414">
+    <cfRule type="containsBlanks" dxfId="52" priority="53">
       <formula>LEN(TRIM(C406))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D399:D405 D407">
-    <cfRule type="containsBlanks" dxfId="63" priority="60">
-      <formula>LEN(TRIM(D399))=0</formula>
+  <conditionalFormatting sqref="E407">
+    <cfRule type="containsBlanks" dxfId="51" priority="52">
+      <formula>LEN(TRIM(E407))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D406">
-    <cfRule type="containsBlanks" dxfId="62" priority="59">
-      <formula>LEN(TRIM(D406))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E399:E407">
-    <cfRule type="containsBlanks" dxfId="61" priority="58">
-      <formula>LEN(TRIM(E399))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F399:F407">
-    <cfRule type="containsBlanks" dxfId="60" priority="57">
-      <formula>LEN(TRIM(F399))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G401:G407">
-    <cfRule type="containsBlanks" dxfId="59" priority="56">
-      <formula>LEN(TRIM(G401))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G398">
-    <cfRule type="containsBlanks" dxfId="58" priority="55">
-      <formula>LEN(TRIM(G398))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H400">
-    <cfRule type="containsBlanks" dxfId="57" priority="54">
-      <formula>LEN(TRIM(H400))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I398:K407">
-    <cfRule type="containsBlanks" dxfId="56" priority="53">
-      <formula>LEN(TRIM(I398))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G197">
-    <cfRule type="containsBlanks" dxfId="55" priority="52">
-      <formula>LEN(TRIM(G197))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C410 C408:G408 K408:K413 K416">
-    <cfRule type="containsBlanks" dxfId="54" priority="51">
-      <formula>LEN(TRIM(C408))=0</formula>
+  <conditionalFormatting sqref="E408">
+    <cfRule type="containsBlanks" dxfId="50" priority="51">
+      <formula>LEN(TRIM(E408))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E409">
-    <cfRule type="containsBlanks" dxfId="53" priority="50">
+    <cfRule type="containsBlanks" dxfId="49" priority="50">
       <formula>LEN(TRIM(E409))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E410">
-    <cfRule type="containsBlanks" dxfId="52" priority="49">
+    <cfRule type="containsBlanks" dxfId="48" priority="49">
       <formula>LEN(TRIM(E410))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E411">
-    <cfRule type="containsBlanks" dxfId="51" priority="48">
+    <cfRule type="containsBlanks" dxfId="47" priority="48">
       <formula>LEN(TRIM(E411))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E412">
-    <cfRule type="containsBlanks" dxfId="50" priority="47">
-      <formula>LEN(TRIM(E412))=0</formula>
+  <conditionalFormatting sqref="A406:B406">
+    <cfRule type="containsBlanks" dxfId="46" priority="47">
+      <formula>LEN(TRIM(A406))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E413">
-    <cfRule type="containsBlanks" dxfId="49" priority="46">
-      <formula>LEN(TRIM(E413))=0</formula>
+  <conditionalFormatting sqref="A407:B407">
+    <cfRule type="containsBlanks" dxfId="45" priority="46">
+      <formula>LEN(TRIM(A407))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A408:B408">
-    <cfRule type="containsBlanks" dxfId="48" priority="45">
+    <cfRule type="containsBlanks" dxfId="44" priority="45">
       <formula>LEN(TRIM(A408))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A409:B409">
-    <cfRule type="containsBlanks" dxfId="47" priority="44">
+    <cfRule type="containsBlanks" dxfId="43" priority="44">
       <formula>LEN(TRIM(A409))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A410:B410">
-    <cfRule type="containsBlanks" dxfId="46" priority="43">
+    <cfRule type="containsBlanks" dxfId="42" priority="43">
       <formula>LEN(TRIM(A410))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A411:B411">
-    <cfRule type="containsBlanks" dxfId="45" priority="42">
+    <cfRule type="containsBlanks" dxfId="41" priority="42">
       <formula>LEN(TRIM(A411))=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D407">
+    <cfRule type="containsBlanks" dxfId="40" priority="41">
+      <formula>LEN(TRIM(D407))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D409">
+    <cfRule type="containsBlanks" dxfId="39" priority="40">
+      <formula>LEN(TRIM(D409))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D410">
+    <cfRule type="containsBlanks" dxfId="38" priority="39">
+      <formula>LEN(TRIM(D410))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C407">
+    <cfRule type="containsBlanks" dxfId="37" priority="38">
+      <formula>LEN(TRIM(C407))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C409">
+    <cfRule type="containsBlanks" dxfId="36" priority="37">
+      <formula>LEN(TRIM(C409))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C410">
+    <cfRule type="containsBlanks" dxfId="35" priority="36">
+      <formula>LEN(TRIM(C410))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C411">
+    <cfRule type="containsBlanks" dxfId="34" priority="35">
+      <formula>LEN(TRIM(C411))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F407">
+    <cfRule type="containsBlanks" dxfId="33" priority="34">
+      <formula>LEN(TRIM(F407))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F408">
+    <cfRule type="containsBlanks" dxfId="32" priority="33">
+      <formula>LEN(TRIM(F408))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F409">
+    <cfRule type="containsBlanks" dxfId="31" priority="32">
+      <formula>LEN(TRIM(F409))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F410">
+    <cfRule type="containsBlanks" dxfId="30" priority="31">
+      <formula>LEN(TRIM(F410))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F411">
+    <cfRule type="containsBlanks" dxfId="29" priority="30">
+      <formula>LEN(TRIM(F411))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H406">
+    <cfRule type="containsBlanks" dxfId="28" priority="29">
+      <formula>LEN(TRIM(H406))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H407">
+    <cfRule type="containsBlanks" dxfId="27" priority="28">
+      <formula>LEN(TRIM(H407))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H408">
+    <cfRule type="containsBlanks" dxfId="26" priority="27">
+      <formula>LEN(TRIM(H408))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H409">
+    <cfRule type="containsBlanks" dxfId="25" priority="26">
+      <formula>LEN(TRIM(H409))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H410">
+    <cfRule type="containsBlanks" dxfId="24" priority="25">
+      <formula>LEN(TRIM(H410))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H411">
+    <cfRule type="containsBlanks" dxfId="23" priority="24">
+      <formula>LEN(TRIM(H411))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G407">
+    <cfRule type="containsBlanks" dxfId="22" priority="23">
+      <formula>LEN(TRIM(G407))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G408">
+    <cfRule type="containsBlanks" dxfId="21" priority="22">
+      <formula>LEN(TRIM(G408))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G409">
+    <cfRule type="containsBlanks" dxfId="20" priority="21">
+      <formula>LEN(TRIM(G409))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G410">
+    <cfRule type="containsBlanks" dxfId="19" priority="20">
+      <formula>LEN(TRIM(G410))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G411">
+    <cfRule type="containsBlanks" dxfId="18" priority="19">
+      <formula>LEN(TRIM(G411))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K412:K413">
+    <cfRule type="containsBlanks" dxfId="17" priority="18">
+      <formula>LEN(TRIM(K412))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A412:B412">
-    <cfRule type="containsBlanks" dxfId="44" priority="41">
+    <cfRule type="containsBlanks" dxfId="16" priority="17">
       <formula>LEN(TRIM(A412))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A413:B413">
-    <cfRule type="containsBlanks" dxfId="43" priority="40">
+  <conditionalFormatting sqref="A413:B413 A414:A427">
+    <cfRule type="containsBlanks" dxfId="15" priority="16">
       <formula>LEN(TRIM(A413))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D409">
-    <cfRule type="containsBlanks" dxfId="42" priority="39">
-      <formula>LEN(TRIM(D409))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D411">
-    <cfRule type="containsBlanks" dxfId="41" priority="38">
-      <formula>LEN(TRIM(D411))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D412">
-    <cfRule type="containsBlanks" dxfId="40" priority="37">
-      <formula>LEN(TRIM(D412))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C409">
-    <cfRule type="containsBlanks" dxfId="39" priority="36">
-      <formula>LEN(TRIM(C409))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C411">
-    <cfRule type="containsBlanks" dxfId="38" priority="35">
-      <formula>LEN(TRIM(C411))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C412">
-    <cfRule type="containsBlanks" dxfId="37" priority="34">
+    <cfRule type="containsBlanks" dxfId="14" priority="15">
       <formula>LEN(TRIM(C412))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C413">
-    <cfRule type="containsBlanks" dxfId="36" priority="33">
+    <cfRule type="containsBlanks" dxfId="13" priority="14">
       <formula>LEN(TRIM(C413))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F409">
-    <cfRule type="containsBlanks" dxfId="35" priority="32">
-      <formula>LEN(TRIM(F409))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F410">
-    <cfRule type="containsBlanks" dxfId="34" priority="31">
-      <formula>LEN(TRIM(F410))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F411">
-    <cfRule type="containsBlanks" dxfId="33" priority="30">
-      <formula>LEN(TRIM(F411))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F412">
-    <cfRule type="containsBlanks" dxfId="32" priority="29">
-      <formula>LEN(TRIM(F412))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F413">
-    <cfRule type="containsBlanks" dxfId="31" priority="28">
-      <formula>LEN(TRIM(F413))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H408">
-    <cfRule type="containsBlanks" dxfId="30" priority="27">
-      <formula>LEN(TRIM(H408))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H409">
-    <cfRule type="containsBlanks" dxfId="29" priority="26">
-      <formula>LEN(TRIM(H409))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H410">
-    <cfRule type="containsBlanks" dxfId="28" priority="25">
-      <formula>LEN(TRIM(H410))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H411">
-    <cfRule type="containsBlanks" dxfId="27" priority="24">
-      <formula>LEN(TRIM(H411))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H412">
-    <cfRule type="containsBlanks" dxfId="26" priority="23">
-      <formula>LEN(TRIM(H412))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H413">
-    <cfRule type="containsBlanks" dxfId="25" priority="22">
-      <formula>LEN(TRIM(H413))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G409">
-    <cfRule type="containsBlanks" dxfId="24" priority="21">
-      <formula>LEN(TRIM(G409))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G410">
-    <cfRule type="containsBlanks" dxfId="23" priority="20">
-      <formula>LEN(TRIM(G410))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G411">
-    <cfRule type="containsBlanks" dxfId="22" priority="19">
-      <formula>LEN(TRIM(G411))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G412">
-    <cfRule type="containsBlanks" dxfId="21" priority="18">
-      <formula>LEN(TRIM(G412))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G413">
-    <cfRule type="containsBlanks" dxfId="20" priority="17">
-      <formula>LEN(TRIM(G413))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K414:K415">
-    <cfRule type="containsBlanks" dxfId="19" priority="16">
-      <formula>LEN(TRIM(K414))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A414:B414">
-    <cfRule type="containsBlanks" dxfId="18" priority="15">
-      <formula>LEN(TRIM(A414))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A415:B415 A416:A429">
-    <cfRule type="containsBlanks" dxfId="17" priority="14">
-      <formula>LEN(TRIM(A415))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C414">
-    <cfRule type="containsBlanks" dxfId="16" priority="13">
-      <formula>LEN(TRIM(C414))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C415">
-    <cfRule type="containsBlanks" dxfId="15" priority="12">
-      <formula>LEN(TRIM(C415))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A8:K8">
-    <cfRule type="containsBlanks" dxfId="14" priority="11">
+    <cfRule type="containsBlanks" dxfId="12" priority="13">
       <formula>LEN(TRIM(A8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:K7">
-    <cfRule type="containsBlanks" dxfId="12" priority="10">
+    <cfRule type="containsBlanks" dxfId="11" priority="12">
       <formula>LEN(TRIM(F7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:F6 I6:K6">
-    <cfRule type="containsBlanks" dxfId="11" priority="9">
+    <cfRule type="containsBlanks" dxfId="10" priority="11">
       <formula>LEN(TRIM(A6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:K5">
-    <cfRule type="containsBlanks" dxfId="8" priority="8">
+    <cfRule type="containsBlanks" dxfId="9" priority="10">
       <formula>LEN(TRIM(A5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:K4">
-    <cfRule type="containsBlanks" dxfId="7" priority="7">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:K3">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B416:B429">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(B416))=0</formula>
+  <conditionalFormatting sqref="B414:B429">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(B414))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K417:K429">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(K417))=0</formula>
+  <conditionalFormatting sqref="K415:K427">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(K415))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="4" priority="4">
       <formula>LEN(TRIM(H6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(G6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K428">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
+      <formula>LEN(TRIM(K428))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D429:K429">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(D429))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18242,7 +18278,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I17">
-    <cfRule type="containsBlanks" dxfId="6" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(I17))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18275,10 +18311,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15001D91-9CB8-4DAB-A1A3-2C399064AEE1}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18315,6 +18351,22 @@
         <v>30</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>522</v>
+      </c>
+      <c r="C4" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>526</v>
+      </c>
+      <c r="C5" t="s">
+        <v>529</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated read from excel sheet so it now selects by column name instead of index. Therefore, the input is allowed to have extra columns now.
</commit_message>
<xml_diff>
--- a/test_constraints.xlsx
+++ b/test_constraints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HumeD\PycharmProjects\Data_Profile_Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECD99EA-8AE0-4CA7-A52D-935F0A5100BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC697C0-2B2E-4201-933F-5FB1D2C9EEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{D2E9D144-5D6F-4AC1-9DA3-D4FF634D9598}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{D2E9D144-5D6F-4AC1-9DA3-D4FF634D9598}"/>
   </bookViews>
   <sheets>
     <sheet name="Constraint Set Definitions" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3059" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3080" uniqueCount="544">
   <si>
     <t>Constraint_Set_Name</t>
   </si>
@@ -1637,6 +1637,42 @@
   </si>
   <si>
     <t>X,X</t>
+  </si>
+  <si>
+    <t>Empty Data Sets</t>
+  </si>
+  <si>
+    <t>Mismatching Relative: Too Few Columns</t>
+  </si>
+  <si>
+    <t>Mismatching Relative: Too Many Columns</t>
+  </si>
+  <si>
+    <t>Main: Matching Data Sets</t>
+  </si>
+  <si>
+    <t>Main: Different Data Sets</t>
+  </si>
+  <si>
+    <t>STS2</t>
+  </si>
+  <si>
+    <t>STS3</t>
+  </si>
+  <si>
+    <t>STS4</t>
+  </si>
+  <si>
+    <t>Main: Empty Secondary Data Set</t>
+  </si>
+  <si>
+    <t>C:/sandbox/data/raw/Data_Profile_Tester/sts2.dat</t>
+  </si>
+  <si>
+    <t>C:/sandbox/data/raw/Data_Profile_Tester/sts3.dat</t>
+  </si>
+  <si>
+    <t>C:/sandbox/data/raw/Data_Profile_Tester/sts4.dat</t>
   </si>
 </sst>
 </file>
@@ -2597,10 +2633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8623B9B9-CDA9-468A-BDFA-05B32D11770D}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2617,7 +2653,7 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -2630,82 +2666,122 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
+        <v>532</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>530</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>530</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>523</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2</v>
+        <v>535</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>530</v>
+        <v>28</v>
       </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="B4" s="5">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2765,7 +2841,7 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2801,13 +2877,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -2828,13 +2904,20 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2846,7 +2929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E86614-3B97-43D1-B6C4-36CEB2305CDA}">
   <dimension ref="A1:K429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
+    <sheetView topLeftCell="A384" workbookViewId="0">
       <selection activeCell="A389" sqref="A389:XFD389"/>
     </sheetView>
   </sheetViews>
@@ -18311,16 +18394,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15001D91-9CB8-4DAB-A1A3-2C399064AEE1}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18337,18 +18420,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>526</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>529</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -18361,10 +18444,34 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>526</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>529</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>537</v>
+      </c>
+      <c r="C6" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>538</v>
+      </c>
+      <c r="C7" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>539</v>
+      </c>
+      <c r="C8" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
i have eliminated most of the ERR tests that shouldnt have made it all the way through. 83 / 229 valid test are making it through atm
</commit_message>
<xml_diff>
--- a/test_constraints.xlsx
+++ b/test_constraints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HumeD\PycharmProjects\Data_Profile_Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC697C0-2B2E-4201-933F-5FB1D2C9EEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2296BE4F-C588-48F7-A627-A215D091ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{D2E9D144-5D6F-4AC1-9DA3-D4FF634D9598}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{D2E9D144-5D6F-4AC1-9DA3-D4FF634D9598}"/>
   </bookViews>
   <sheets>
     <sheet name="Constraint Set Definitions" sheetId="1" r:id="rId1"/>
@@ -2635,7 +2635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8623B9B9-CDA9-468A-BDFA-05B32D11770D}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2929,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E86614-3B97-43D1-B6C4-36CEB2305CDA}">
   <dimension ref="A1:K429"/>
   <sheetViews>
-    <sheetView topLeftCell="A384" workbookViewId="0">
-      <selection activeCell="A389" sqref="A389:XFD389"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>